<commit_message>
Minor fixes + readme update
Minor fixes to chapters 6, 7, 9, and 10 and upate of readme file.
</commit_message>
<xml_diff>
--- a/IndicatorList.xlsx
+++ b/IndicatorList.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33697\ICF\Analysis - Shared Resources\Code\DHS-Indicators-Stata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="6_{62BF7E7C-45DE-4506-B34F-5C16B6014826}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{3EB8B577-1C2B-4819-B62C-BDF606B693DF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10224" windowHeight="3504"/>
+    <workbookView xWindow="-25252" yWindow="-118" windowWidth="25370" windowHeight="13759" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH2PH" sheetId="17" r:id="rId1"/>
@@ -34,18 +35,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="1322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="1324">
   <si>
     <t>Chapter</t>
   </si>
@@ -4012,12 +4007,18 @@
   </si>
   <si>
     <t xml:space="preserve">Master file for the women's empowerment chapter. The master file will call the do files listed below and the WE_tables.do file not listed here. The tables do file will produce excel tables of the indicators. Some of the do files will also produce tables as indicated in the notes below. Please check for country specific variations. </t>
+  </si>
+  <si>
+    <t>CH_STOOL.do</t>
+  </si>
+  <si>
+    <t>Do file will drop observations. Please see notes in do file.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4183,6 +4184,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4205,16 +4215,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4495,28 +4496,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F127"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
@@ -4527,7 +4528,7 @@
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4547,21 +4548,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>835</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>836</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>837</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="17"/>
       <c r="C3" s="19"/>
@@ -4569,7 +4570,7 @@
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="17"/>
       <c r="B4" s="17" t="s">
         <v>838</v>
@@ -4585,7 +4586,7 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17" t="s">
@@ -4599,7 +4600,7 @@
       </c>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17" t="s">
@@ -4613,7 +4614,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17" t="s">
@@ -4627,7 +4628,7 @@
       </c>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
@@ -4637,7 +4638,7 @@
       </c>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17" t="s">
@@ -4651,7 +4652,7 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17" t="s">
@@ -4665,7 +4666,7 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17" t="s">
@@ -4679,7 +4680,7 @@
       </c>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17" t="s">
@@ -4693,7 +4694,7 @@
       </c>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17" t="s">
@@ -4707,7 +4708,7 @@
       </c>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
@@ -4717,7 +4718,7 @@
       </c>
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17" t="s">
@@ -4731,7 +4732,7 @@
       </c>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17" t="s">
@@ -4745,7 +4746,7 @@
       </c>
       <c r="F16" s="17"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17" t="s">
@@ -4759,7 +4760,7 @@
       </c>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
@@ -4769,7 +4770,7 @@
       </c>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17" t="s">
@@ -4959,7 +4960,7 @@
       </c>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17" t="s">
@@ -5001,7 +5002,7 @@
       </c>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
       <c r="B35" s="17"/>
       <c r="C35" s="17" t="s">
@@ -5028,7 +5029,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A37" s="17"/>
       <c r="B37" s="17"/>
       <c r="C37" s="17" t="s">
@@ -5041,7 +5042,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="17"/>
       <c r="B38" s="17"/>
       <c r="C38" s="17" t="s">
@@ -5145,7 +5146,7 @@
       </c>
       <c r="F45" s="17"/>
     </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A46" s="17"/>
       <c r="B46" s="17"/>
       <c r="C46" s="17" t="s">
@@ -5185,7 +5186,7 @@
       </c>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="17" t="s">
@@ -5211,7 +5212,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A51" s="17"/>
       <c r="B51" s="17"/>
       <c r="C51" s="17" t="s">
@@ -5225,7 +5226,7 @@
       </c>
       <c r="F51" s="17"/>
     </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17" t="s">
@@ -5529,7 +5530,7 @@
       </c>
       <c r="F74" s="17"/>
     </row>
-    <row r="75" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="17"/>
       <c r="B75" s="17"/>
       <c r="C75" s="17" t="s">
@@ -5607,7 +5608,7 @@
       </c>
       <c r="F80" s="17"/>
     </row>
-    <row r="81" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="17"/>
       <c r="B81" s="17"/>
       <c r="C81" s="17" t="s">
@@ -6044,7 +6045,7 @@
       </c>
       <c r="F112" s="17"/>
     </row>
-    <row r="113" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="15.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="17"/>
       <c r="B113" s="17"/>
       <c r="C113" s="17" t="s">
@@ -6071,7 +6072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="17"/>
       <c r="B115" s="17"/>
       <c r="C115" s="17" t="s">
@@ -6115,7 +6116,7 @@
       </c>
       <c r="F117" s="17"/>
     </row>
-    <row r="118" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="17"/>
       <c r="B118" s="17"/>
       <c r="C118" s="17" t="s">
@@ -6211,14 +6212,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="1" customWidth="1"/>
@@ -6229,7 +6230,7 @@
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6249,19 +6250,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1048</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>1049</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>1050</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
@@ -6273,7 +6274,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="17"/>
       <c r="B4" s="17" t="s">
         <v>1052</v>
@@ -6291,7 +6292,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17" t="s">
@@ -6307,7 +6308,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17" t="s">
@@ -6323,7 +6324,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17" t="s">
@@ -6415,7 +6416,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
@@ -6425,7 +6426,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
@@ -6459,7 +6460,7 @@
       <c r="E16" s="17" t="s">
         <v>1084</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="31" t="s">
         <v>1085</v>
       </c>
     </row>
@@ -6473,7 +6474,7 @@
         <v>1087</v>
       </c>
       <c r="E17" s="17"/>
-      <c r="F17" s="28"/>
+      <c r="F17" s="31"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
@@ -6487,7 +6488,7 @@
       <c r="E18" s="17"/>
       <c r="F18" s="20"/>
     </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -6525,7 +6526,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
@@ -6549,11 +6550,11 @@
       <c r="E23" s="17" t="s">
         <v>972</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="32" t="s">
         <v>1099</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="29" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="17"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17" t="s">
@@ -6565,9 +6566,9 @@
       <c r="E24" s="17" t="s">
         <v>972</v>
       </c>
-      <c r="F24" s="29"/>
-    </row>
-    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="F24" s="32"/>
+    </row>
+    <row r="25" spans="1:6" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -6579,7 +6580,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="26" t="s">
         <v>1103</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -6597,7 +6598,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="17"/>
-      <c r="B27" s="23"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="1" t="s">
         <v>1107</v>
       </c>
@@ -6613,7 +6614,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
-      <c r="B28" s="23"/>
+      <c r="B28" s="26"/>
       <c r="C28" s="1" t="s">
         <v>1109</v>
       </c>
@@ -6629,7 +6630,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
-      <c r="B29" s="23"/>
+      <c r="B29" s="26"/>
       <c r="C29" s="17" t="s">
         <v>1111</v>
       </c>
@@ -6643,7 +6644,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
-      <c r="B30" s="23"/>
+      <c r="B30" s="26"/>
       <c r="C30" s="17" t="s">
         <v>1113</v>
       </c>
@@ -6657,7 +6658,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
-      <c r="B31" s="23"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="17" t="s">
         <v>1115</v>
       </c>
@@ -6669,7 +6670,7 @@
       </c>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -6723,7 +6724,7 @@
       </c>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
@@ -6765,7 +6766,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
       <c r="C39" s="17" t="s">
@@ -6809,7 +6810,7 @@
       </c>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A42" s="17"/>
       <c r="B42" s="17"/>
       <c r="C42" s="17" t="s">
@@ -6823,7 +6824,7 @@
       </c>
       <c r="F42" s="17"/>
     </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
       <c r="C43" s="17" t="s">
@@ -6837,7 +6838,7 @@
       </c>
       <c r="F43" s="17"/>
     </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A44" s="17"/>
       <c r="B44" s="17"/>
       <c r="C44" s="17" t="s">
@@ -6865,7 +6866,7 @@
       </c>
       <c r="F45" s="17"/>
     </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A46" s="17"/>
       <c r="B46" s="17"/>
       <c r="C46" s="17" t="s">
@@ -6893,7 +6894,7 @@
       </c>
       <c r="F47" s="17"/>
     </row>
-    <row r="48" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17" t="s">
@@ -6921,7 +6922,7 @@
       </c>
       <c r="F49" s="17"/>
     </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A50" s="17"/>
       <c r="B50" s="17"/>
       <c r="C50" s="17" t="s">
@@ -6943,7 +6944,7 @@
       <c r="E51" s="17"/>
       <c r="F51" s="17"/>
     </row>
-    <row r="52" spans="1:6" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="37.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17" t="s">
@@ -7225,24 +7226,24 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.44140625" customWidth="1"/>
     <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
     <col min="4" max="4" width="113.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.6640625" style="30" customWidth="1"/>
+    <col min="6" max="6" width="55.6640625" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -7262,691 +7263,691 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="47.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1178</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>1179</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>1180</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" spans="1:6" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="31" t="s">
+    <row r="5" spans="1:6" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B5" s="24" t="s">
         <v>1181</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="24" t="s">
         <v>1182</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="24" t="s">
         <v>1183</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="31" t="s">
+    <row r="6" spans="1:6" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C6" s="24" t="s">
         <v>1184</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="24" t="s">
         <v>1189</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="31" t="s">
+    <row r="7" spans="1:6" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C7" s="24" t="s">
         <v>1185</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="24" t="s">
         <v>1186</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="31" t="s">
+    <row r="8" spans="1:6" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C8" s="24" t="s">
         <v>1187</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="24" t="s">
         <v>1188</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="31" t="s">
+    <row r="9" spans="1:6" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C9" s="24" t="s">
         <v>1190</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="24" t="s">
         <v>1191</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="31" t="s">
+    <row r="10" spans="1:6" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C10" s="24" t="s">
         <v>1192</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="24" t="s">
         <v>1193</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="31" t="s">
+    <row r="11" spans="1:6" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C11" s="24" t="s">
         <v>1194</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="24" t="s">
         <v>1195</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="31" t="s">
+    <row r="12" spans="1:6" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C12" s="24" t="s">
         <v>1196</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="24" t="s">
         <v>1197</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" s="31" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="C13" s="31" t="s">
+    <row r="13" spans="1:6" s="24" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C13" s="24" t="s">
         <v>1198</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="24" t="s">
         <v>1199</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>1200</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="31" t="s">
+    <row r="14" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="24" t="s">
         <v>1201</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="24" t="s">
         <v>1202</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="31" t="s">
+    <row r="15" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="24" t="s">
         <v>1203</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="24" t="s">
         <v>1204</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="31" t="s">
+    <row r="17" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="24" t="s">
         <v>1205</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="24" t="s">
         <v>1210</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="31" t="s">
+    <row r="18" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="24" t="s">
         <v>1206</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="24" t="s">
         <v>1211</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="31" t="s">
+    <row r="19" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="24" t="s">
         <v>1207</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="24" t="s">
         <v>1212</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="31" t="s">
+    <row r="20" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="24" t="s">
         <v>1208</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="24" t="s">
         <v>1213</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="31" t="s">
+    <row r="21" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="24" t="s">
         <v>1209</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="24" t="s">
         <v>1214</v>
       </c>
-      <c r="E21" s="31" t="s">
+      <c r="E21" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="31" t="s">
+    <row r="23" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="24" t="s">
         <v>1215</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="24" t="s">
         <v>1216</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="24" t="s">
         <v>1217</v>
       </c>
-      <c r="E23" s="31" t="s">
+      <c r="E23" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="31" t="s">
+    <row r="24" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="24" t="s">
         <v>1218</v>
       </c>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="24" t="s">
         <v>1219</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="31" t="s">
+    <row r="25" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="24" t="s">
         <v>1220</v>
       </c>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="24" t="s">
         <v>1221</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="E25" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="31" t="s">
+    <row r="27" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="24" t="s">
         <v>1222</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="24" t="s">
         <v>1223</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="24" t="s">
         <v>1224</v>
       </c>
-      <c r="E27" s="31" t="s">
+      <c r="E27" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="32" t="s">
+      <c r="F27" s="33" t="s">
         <v>1225</v>
       </c>
     </row>
-    <row r="28" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="31" t="s">
+    <row r="28" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="24" t="s">
         <v>1226</v>
       </c>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="24" t="s">
         <v>1227</v>
       </c>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="32"/>
-    </row>
-    <row r="29" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="31" t="s">
+      <c r="F28" s="33"/>
+    </row>
+    <row r="29" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="24" t="s">
         <v>1228</v>
       </c>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="24" t="s">
         <v>1229</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F29" s="32"/>
-    </row>
-    <row r="30" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="31" t="s">
+      <c r="F29" s="33"/>
+    </row>
+    <row r="30" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="24" t="s">
         <v>1230</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D30" s="24" t="s">
         <v>1231</v>
       </c>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="32"/>
-    </row>
-    <row r="31" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="33"/>
+    </row>
+    <row r="31" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="31" t="s">
+    <row r="32" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="24" t="s">
         <v>1232</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="24" t="s">
         <v>1235</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="24" t="s">
         <v>22</v>
       </c>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="31" t="s">
+    <row r="33" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="24" t="s">
         <v>1233</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="24" t="s">
         <v>1236</v>
       </c>
-      <c r="E33" s="31" t="s">
+      <c r="E33" s="24" t="s">
         <v>22</v>
       </c>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="31" t="s">
+    <row r="34" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="24" t="s">
         <v>1234</v>
       </c>
-      <c r="D34" s="31" t="s">
+      <c r="D34" s="24" t="s">
         <v>1237</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E34" s="24" t="s">
         <v>22</v>
       </c>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="31" t="s">
+    <row r="36" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="24" t="s">
         <v>1238</v>
       </c>
-      <c r="C36" s="31" t="s">
+      <c r="C36" s="24" t="s">
         <v>1239</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="24" t="s">
         <v>1240</v>
       </c>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="31" t="s">
+    <row r="37" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="24" t="s">
         <v>1241</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="24" t="s">
         <v>1242</v>
       </c>
-      <c r="E37" s="31" t="s">
+      <c r="E37" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="31" t="s">
+    <row r="38" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C38" s="24" t="s">
         <v>1243</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D38" s="24" t="s">
         <v>1244</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="31" t="s">
+    <row r="39" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="24" t="s">
         <v>1245</v>
       </c>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="24" t="s">
         <v>1246</v>
       </c>
-      <c r="E39" s="31" t="s">
+      <c r="E39" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="31" t="s">
+    <row r="41" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="24" t="s">
         <v>1247</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="24" t="s">
         <v>1252</v>
       </c>
-      <c r="E41" s="31" t="s">
+      <c r="E41" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="31" t="s">
+    <row r="42" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="24" t="s">
         <v>1248</v>
       </c>
-      <c r="D42" s="31" t="s">
+      <c r="D42" s="24" t="s">
         <v>1251</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F42" s="22"/>
     </row>
-    <row r="43" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="31" t="s">
+    <row r="43" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="24" t="s">
         <v>1249</v>
       </c>
-      <c r="D43" s="31" t="s">
+      <c r="D43" s="24" t="s">
         <v>1250</v>
       </c>
-      <c r="E43" s="31" t="s">
+      <c r="E43" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F43" s="22"/>
     </row>
-    <row r="44" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="31" t="s">
+    <row r="44" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="24" t="s">
         <v>1253</v>
       </c>
-      <c r="D44" s="31" t="s">
+      <c r="D44" s="24" t="s">
         <v>1254</v>
       </c>
-      <c r="E44" s="31" t="s">
+      <c r="E44" s="24" t="s">
         <v>17</v>
       </c>
       <c r="F44" s="22"/>
     </row>
-    <row r="45" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F45" s="22"/>
     </row>
-    <row r="46" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="31" t="s">
+    <row r="46" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="24" t="s">
         <v>1272</v>
       </c>
-      <c r="D46" s="31" t="s">
+      <c r="D46" s="24" t="s">
         <v>1271</v>
       </c>
-      <c r="E46" s="31" t="s">
+      <c r="E46" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F46" s="22"/>
     </row>
-    <row r="47" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="31" t="s">
+    <row r="47" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="24" t="s">
         <v>1273</v>
       </c>
-      <c r="D47" s="31" t="s">
+      <c r="D47" s="24" t="s">
         <v>1274</v>
       </c>
-      <c r="E47" s="31" t="s">
+      <c r="E47" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F47" s="22"/>
     </row>
-    <row r="48" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F48" s="22"/>
     </row>
-    <row r="49" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="31" t="s">
+    <row r="49" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="24" t="s">
         <v>1255</v>
       </c>
-      <c r="C49" s="31" t="s">
+      <c r="C49" s="24" t="s">
         <v>1257</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="24" t="s">
         <v>1256</v>
       </c>
-      <c r="E49" s="31" t="s">
+      <c r="E49" s="24" t="s">
         <v>22</v>
       </c>
       <c r="F49" s="22"/>
     </row>
-    <row r="50" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="31" t="s">
+    <row r="50" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="24" t="s">
         <v>1258</v>
       </c>
-      <c r="D50" s="31" t="s">
+      <c r="D50" s="24" t="s">
         <v>1259</v>
       </c>
-      <c r="E50" s="31" t="s">
+      <c r="E50" s="24" t="s">
         <v>22</v>
       </c>
       <c r="F50" s="22"/>
     </row>
-    <row r="51" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F51" s="22"/>
     </row>
-    <row r="52" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="31" t="s">
+    <row r="52" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="24" t="s">
         <v>1260</v>
       </c>
-      <c r="C52" s="31" t="s">
+      <c r="C52" s="24" t="s">
         <v>1261</v>
       </c>
-      <c r="D52" s="31" t="s">
+      <c r="D52" s="24" t="s">
         <v>1262</v>
       </c>
-      <c r="E52" s="31" t="s">
+      <c r="E52" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F52" s="22"/>
     </row>
-    <row r="53" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="31" t="s">
+    <row r="53" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="24" t="s">
         <v>1263</v>
       </c>
-      <c r="D53" s="31" t="s">
+      <c r="D53" s="24" t="s">
         <v>1264</v>
       </c>
-      <c r="E53" s="31" t="s">
+      <c r="E53" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F53" s="22"/>
     </row>
-    <row r="54" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="31" t="s">
+    <row r="54" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="24" t="s">
         <v>1265</v>
       </c>
-      <c r="D54" s="31" t="s">
+      <c r="D54" s="24" t="s">
         <v>1266</v>
       </c>
-      <c r="E54" s="31" t="s">
+      <c r="E54" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F54" s="22"/>
     </row>
-    <row r="55" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="31" t="s">
+    <row r="55" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="24" t="s">
         <v>1267</v>
       </c>
-      <c r="D55" s="31" t="s">
+      <c r="D55" s="24" t="s">
         <v>1268</v>
       </c>
-      <c r="E55" s="31" t="s">
+      <c r="E55" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F55" s="22"/>
     </row>
-    <row r="56" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="31" t="s">
+    <row r="56" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="24" t="s">
         <v>1269</v>
       </c>
-      <c r="D56" s="31" t="s">
+      <c r="D56" s="24" t="s">
         <v>1270</v>
       </c>
-      <c r="E56" s="31" t="s">
+      <c r="E56" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F56" s="22"/>
     </row>
-    <row r="57" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F57" s="22"/>
     </row>
-    <row r="58" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="31" t="s">
+    <row r="58" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="24" t="s">
         <v>1275</v>
       </c>
-      <c r="C58" s="31" t="s">
+      <c r="C58" s="24" t="s">
         <v>1276</v>
       </c>
-      <c r="D58" s="31" t="s">
+      <c r="D58" s="24" t="s">
         <v>1277</v>
       </c>
-      <c r="E58" s="31" t="s">
+      <c r="E58" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F58" s="22"/>
     </row>
-    <row r="59" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C59" s="31" t="s">
+    <row r="59" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C59" s="24" t="s">
         <v>1278</v>
       </c>
-      <c r="D59" s="31" t="s">
+      <c r="D59" s="24" t="s">
         <v>1279</v>
       </c>
-      <c r="E59" s="31" t="s">
+      <c r="E59" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F59" s="22"/>
     </row>
-    <row r="60" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="31" t="s">
+    <row r="60" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="24" t="s">
         <v>1280</v>
       </c>
-      <c r="D60" s="31" t="s">
+      <c r="D60" s="24" t="s">
         <v>1281</v>
       </c>
-      <c r="E60" s="31" t="s">
+      <c r="E60" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F60" s="22"/>
     </row>
-    <row r="61" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C61" s="31" t="s">
+    <row r="61" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="24" t="s">
         <v>1282</v>
       </c>
-      <c r="D61" s="31" t="s">
+      <c r="D61" s="24" t="s">
         <v>1283</v>
       </c>
-      <c r="E61" s="31" t="s">
+      <c r="E61" s="24" t="s">
         <v>12</v>
       </c>
       <c r="F61" s="22"/>
     </row>
-    <row r="62" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F62" s="22"/>
     </row>
-    <row r="63" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F63" s="22"/>
     </row>
-    <row r="64" spans="2:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F64" s="22"/>
     </row>
-    <row r="65" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F65" s="22"/>
     </row>
-    <row r="66" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F66" s="22"/>
     </row>
-    <row r="67" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F67" s="22"/>
     </row>
-    <row r="68" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F68" s="22"/>
     </row>
-    <row r="69" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F69" s="22"/>
     </row>
-    <row r="70" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F70" s="22"/>
     </row>
-    <row r="71" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F71" s="22"/>
     </row>
-    <row r="72" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F72" s="22"/>
     </row>
-    <row r="73" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F73" s="22"/>
     </row>
-    <row r="74" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F74" s="22"/>
     </row>
-    <row r="75" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F75" s="22"/>
     </row>
-    <row r="76" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F76" s="22"/>
     </row>
-    <row r="77" spans="6:6" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="6:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F77" s="22"/>
     </row>
   </sheetData>
@@ -7960,25 +7961,25 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="31" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" style="31" customWidth="1"/>
-    <col min="3" max="3" width="18.77734375" style="31" customWidth="1"/>
-    <col min="4" max="4" width="75.21875" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" style="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" style="24" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" style="24" customWidth="1"/>
+    <col min="4" max="4" width="75.21875" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" style="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.88671875" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="31"/>
+    <col min="7" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -7998,45 +7999,45 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="33" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="47.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>1317</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>1284</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>1320</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="31" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B4" s="24" t="s">
         <v>1285</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="24" t="s">
         <v>1286</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="24" t="s">
         <v>1287</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="24" t="s">
         <v>1288</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="24" t="s">
         <v>1289</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="24" t="s">
         <v>1290</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="24" t="s">
         <v>1291</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="24" t="s">
         <v>1292</v>
       </c>
       <c r="F6" s="22" t="s">
@@ -8044,120 +8045,120 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="24" t="s">
         <v>1294</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="24" t="s">
         <v>1295</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="24" t="s">
         <v>1292</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="33" t="s">
         <v>1293</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="24" t="s">
         <v>1296</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="24" t="s">
         <v>1297</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="24" t="s">
         <v>1292</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="24" t="s">
         <v>1298</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="24" t="s">
         <v>1299</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="24" t="s">
         <v>1292</v>
       </c>
-      <c r="F9" s="32"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C11" s="31" t="s">
+      <c r="F9" s="33"/>
+    </row>
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C11" s="24" t="s">
         <v>1300</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="24" t="s">
         <v>1302</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="24" t="s">
         <v>1292</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C12" s="31" t="s">
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C12" s="24" t="s">
         <v>1301</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="24" t="s">
         <v>1303</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="24" t="s">
         <v>1292</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="31" t="s">
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B14" s="24" t="s">
         <v>1304</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="24" t="s">
         <v>1305</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="24" t="s">
         <v>1306</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="24" t="s">
         <v>1307</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="24" t="s">
         <v>1308</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="24" t="s">
         <v>1309</v>
       </c>
-      <c r="E15" s="31" t="s">
+      <c r="E15" s="24" t="s">
         <v>1307</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="24" t="s">
         <v>1311</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="24" t="s">
         <v>1310</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="24" t="s">
         <v>1307</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="24" t="s">
         <v>1312</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="24" t="s">
         <v>1313</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="E17" s="24" t="s">
         <v>1307</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="24" t="s">
         <v>1314</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="24" t="s">
         <v>1315</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="24" t="s">
         <v>1316</v>
       </c>
     </row>
@@ -8171,14 +8172,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.5546875" customWidth="1"/>
     <col min="2" max="2" width="14.109375" customWidth="1"/>
@@ -8187,7 +8188,7 @@
     <col min="6" max="6" width="38.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8207,19 +8208,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="33" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="47.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>1318</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>1319</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>1321</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8230,56 +8231,56 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
@@ -8290,7 +8291,7 @@
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8317,14 +8318,14 @@
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="17"/>
       <c r="C3" s="18"/>
@@ -8332,7 +8333,7 @@
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="17"/>
       <c r="B4" s="17" t="s">
         <v>9</v>
@@ -8348,7 +8349,7 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17" t="s">
@@ -8362,7 +8363,7 @@
       </c>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17" t="s">
@@ -8376,7 +8377,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17" t="s">
@@ -8390,7 +8391,7 @@
       </c>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17" t="s">
@@ -8404,7 +8405,7 @@
       </c>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17" t="s">
@@ -8418,7 +8419,7 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17" t="s">
@@ -8432,7 +8433,7 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17" t="s">
@@ -8446,7 +8447,7 @@
       </c>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17" t="s">
@@ -8460,7 +8461,7 @@
       </c>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17" t="s">
@@ -8474,7 +8475,7 @@
       </c>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17" t="s">
@@ -8488,7 +8489,7 @@
       </c>
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17" t="s">
@@ -8504,7 +8505,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17" t="s">
@@ -8518,7 +8519,7 @@
       </c>
       <c r="F16" s="17"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
@@ -8526,7 +8527,7 @@
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
       <c r="B18" s="17" t="s">
         <v>40</v>
@@ -8598,7 +8599,7 @@
       </c>
       <c r="F22" s="17"/>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17" t="s">
@@ -8662,14 +8663,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" style="6" customWidth="1"/>
@@ -8680,7 +8681,7 @@
     <col min="7" max="16384" width="8.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -8707,14 +8708,14 @@
       <c r="B2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -8722,7 +8723,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>58</v>
@@ -8740,7 +8741,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
@@ -8756,7 +8757,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
@@ -8772,7 +8773,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
@@ -8788,7 +8789,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
@@ -8804,7 +8805,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
@@ -8820,7 +8821,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
@@ -8836,7 +8837,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
@@ -8852,7 +8853,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
@@ -8868,7 +8869,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -8876,7 +8877,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
         <v>78</v>
@@ -8894,7 +8895,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -8902,7 +8903,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
         <v>81</v>
@@ -8920,7 +8921,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -9379,14 +9380,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="6" customWidth="1"/>
     <col min="2" max="2" width="17.109375" style="6" customWidth="1"/>
@@ -9397,7 +9398,7 @@
     <col min="7" max="16384" width="8.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -9424,14 +9425,14 @@
       <c r="B2" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -9439,7 +9440,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>149</v>
@@ -9455,7 +9456,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
@@ -9469,7 +9470,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
@@ -9511,7 +9512,7 @@
       </c>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -9537,7 +9538,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -9545,7 +9546,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>164</v>
@@ -9561,7 +9562,7 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -9578,14 +9579,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F146"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
@@ -9596,7 +9597,7 @@
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -9616,21 +9617,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="33.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>167</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -9638,7 +9639,7 @@
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="17"/>
       <c r="B4" s="17" t="s">
         <v>170</v>
@@ -9654,7 +9655,7 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17" t="s">
@@ -9668,7 +9669,7 @@
       </c>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17" t="s">
@@ -9682,7 +9683,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17" t="s">
@@ -9696,7 +9697,7 @@
       </c>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17" t="s">
@@ -9710,7 +9711,7 @@
       </c>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17" t="s">
@@ -9724,7 +9725,7 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17" t="s">
@@ -9738,7 +9739,7 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17" t="s">
@@ -9752,7 +9753,7 @@
       </c>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17" t="s">
@@ -9766,7 +9767,7 @@
       </c>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17" t="s">
@@ -9780,7 +9781,7 @@
       </c>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17" t="s">
@@ -9794,7 +9795,7 @@
       </c>
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17" t="s">
@@ -9808,7 +9809,7 @@
       </c>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17" t="s">
@@ -9822,7 +9823,7 @@
       </c>
       <c r="F16" s="17"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17" t="s">
@@ -9836,7 +9837,7 @@
       </c>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17" t="s">
@@ -9998,7 +9999,7 @@
       <c r="E29" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="29" t="s">
         <v>223</v>
       </c>
     </row>
@@ -10014,7 +10015,7 @@
       <c r="E30" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="29"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
@@ -10028,7 +10029,7 @@
       <c r="E31" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="29"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
@@ -10042,7 +10043,7 @@
       <c r="E32" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="26"/>
+      <c r="F32" s="29"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
@@ -10056,7 +10057,7 @@
       <c r="E33" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="26"/>
+      <c r="F33" s="29"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="17"/>
@@ -10070,7 +10071,7 @@
       <c r="E34" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="26"/>
+      <c r="F34" s="29"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
@@ -10084,7 +10085,7 @@
       <c r="E35" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F35" s="26"/>
+      <c r="F35" s="29"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="17"/>
@@ -10098,7 +10099,7 @@
       <c r="E36" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="26"/>
+      <c r="F36" s="29"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="17"/>
@@ -10112,7 +10113,7 @@
       <c r="E37" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="26"/>
+      <c r="F37" s="29"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="17"/>
@@ -10126,7 +10127,7 @@
       <c r="E38" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="26"/>
+      <c r="F38" s="29"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="17"/>
@@ -10140,7 +10141,7 @@
       <c r="E39" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="26"/>
+      <c r="F39" s="29"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="17"/>
@@ -10154,7 +10155,7 @@
       <c r="E40" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F40" s="26"/>
+      <c r="F40" s="29"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="17"/>
@@ -10168,7 +10169,7 @@
       <c r="E41" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F41" s="26"/>
+      <c r="F41" s="29"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="17"/>
@@ -10182,7 +10183,7 @@
       <c r="E42" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F42" s="26"/>
+      <c r="F42" s="29"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="17"/>
@@ -10196,7 +10197,7 @@
       <c r="E43" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F43" s="26"/>
+      <c r="F43" s="29"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="17"/>
@@ -10210,7 +10211,7 @@
       <c r="E44" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="26"/>
+      <c r="F44" s="29"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="17"/>
@@ -10224,7 +10225,7 @@
       <c r="E45" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F45" s="26"/>
+      <c r="F45" s="29"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="17"/>
@@ -10238,7 +10239,7 @@
       <c r="E46" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F46" s="26"/>
+      <c r="F46" s="29"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="17"/>
@@ -10650,7 +10651,7 @@
       <c r="E77" s="17"/>
       <c r="F77" s="17"/>
     </row>
-    <row r="78" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="60.25" x14ac:dyDescent="0.3">
       <c r="A78" s="17"/>
       <c r="B78" s="17"/>
       <c r="C78" s="17" t="s">
@@ -10692,7 +10693,7 @@
       </c>
       <c r="F80" s="17"/>
     </row>
-    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A81" s="17"/>
       <c r="B81" s="17"/>
       <c r="C81" s="17" t="s">
@@ -10706,7 +10707,7 @@
       </c>
       <c r="F81" s="17"/>
     </row>
-    <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A82" s="17"/>
       <c r="B82" s="17"/>
       <c r="C82" s="17" t="s">
@@ -10720,7 +10721,7 @@
       </c>
       <c r="F82" s="17"/>
     </row>
-    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A83" s="17"/>
       <c r="B83" s="17"/>
       <c r="C83" s="17" t="s">
@@ -10734,7 +10735,7 @@
       </c>
       <c r="F83" s="17"/>
     </row>
-    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A84" s="17"/>
       <c r="B84" s="17"/>
       <c r="C84" s="17" t="s">
@@ -10770,7 +10771,7 @@
       <c r="E86" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F86" s="26" t="s">
+      <c r="F86" s="29" t="s">
         <v>329</v>
       </c>
     </row>
@@ -10786,7 +10787,7 @@
       <c r="E87" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F87" s="26"/>
+      <c r="F87" s="29"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="17"/>
@@ -10800,7 +10801,7 @@
       <c r="E88" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F88" s="26"/>
+      <c r="F88" s="29"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="17"/>
@@ -10814,7 +10815,7 @@
       <c r="E89" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F89" s="26"/>
+      <c r="F89" s="29"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="17"/>
@@ -10828,7 +10829,7 @@
       <c r="E90" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F90" s="26"/>
+      <c r="F90" s="29"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="17"/>
@@ -10842,7 +10843,7 @@
       <c r="E91" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F91" s="26"/>
+      <c r="F91" s="29"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="17"/>
@@ -10856,7 +10857,7 @@
       <c r="E92" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F92" s="26"/>
+      <c r="F92" s="29"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="17"/>
@@ -10870,7 +10871,7 @@
       <c r="E93" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F93" s="26"/>
+      <c r="F93" s="29"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="17"/>
@@ -10884,7 +10885,7 @@
       <c r="E94" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F94" s="26"/>
+      <c r="F94" s="29"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="17"/>
@@ -10898,7 +10899,7 @@
       <c r="E95" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F95" s="26"/>
+      <c r="F95" s="29"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="17"/>
@@ -10912,7 +10913,7 @@
       <c r="E96" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F96" s="26"/>
+      <c r="F96" s="29"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="17"/>
@@ -10926,7 +10927,7 @@
       <c r="E97" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F97" s="26"/>
+      <c r="F97" s="29"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="17"/>
@@ -10940,7 +10941,7 @@
       <c r="E98" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F98" s="26"/>
+      <c r="F98" s="29"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="17"/>
@@ -10954,7 +10955,7 @@
       <c r="E99" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F99" s="26"/>
+      <c r="F99" s="29"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="17"/>
@@ -11377,7 +11378,7 @@
       <c r="E131" s="17"/>
       <c r="F131" s="17"/>
     </row>
-    <row r="132" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A132" s="17"/>
       <c r="B132" s="17" t="s">
         <v>413</v>
@@ -11451,7 +11452,7 @@
       </c>
       <c r="F136" s="17"/>
     </row>
-    <row r="137" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" ht="90.35" x14ac:dyDescent="0.3">
       <c r="A137" s="17"/>
       <c r="B137" s="17"/>
       <c r="C137" s="17" t="s">
@@ -11584,14 +11585,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" style="6" customWidth="1"/>
@@ -11602,7 +11603,7 @@
     <col min="7" max="16384" width="8.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -11629,14 +11630,14 @@
       <c r="B2" s="5" t="s">
         <v>441</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="28" t="s">
         <v>442</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -11649,16 +11650,16 @@
       <c r="B4" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="30" t="s">
         <v>444</v>
       </c>
-      <c r="D4" s="27"/>
+      <c r="D4" s="30"/>
       <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -11666,7 +11667,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>445</v>
@@ -11684,7 +11685,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -11692,7 +11693,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>448</v>
@@ -11726,7 +11727,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
@@ -11738,7 +11739,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -11746,7 +11747,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
@@ -11762,7 +11763,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
@@ -11778,7 +11779,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
@@ -11794,7 +11795,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
@@ -11880,7 +11881,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
@@ -11934,7 +11935,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
@@ -11966,7 +11967,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
@@ -12006,7 +12007,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="45.2" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="9" t="s">
@@ -12048,7 +12049,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="10" t="s">
@@ -12064,7 +12065,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="10" t="s">
@@ -12180,7 +12181,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="10" t="s">
@@ -12196,7 +12197,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="10" t="s">
@@ -12212,7 +12213,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="10" t="s">
@@ -12228,7 +12229,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C45" s="10" t="s">
         <v>512</v>
       </c>
@@ -12242,7 +12243,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C46" s="10" t="s">
         <v>514</v>
       </c>
@@ -12280,7 +12281,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="49" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C49" s="10" t="s">
         <v>518</v>
       </c>
@@ -12294,7 +12295,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="50" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C50" s="10" t="s">
         <v>520</v>
       </c>
@@ -12308,7 +12309,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="51" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C51" s="10" t="s">
         <v>522</v>
       </c>
@@ -12322,7 +12323,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="52" spans="3:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="C52" s="10" t="s">
         <v>524</v>
       </c>
@@ -12346,14 +12347,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
@@ -12364,7 +12365,7 @@
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -12384,21 +12385,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>526</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>527</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>528</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -12436,7 +12437,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -12444,7 +12445,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="17" t="s">
         <v>534</v>
@@ -12462,7 +12463,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17" t="s">
@@ -12478,7 +12479,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17" t="s">
@@ -12492,7 +12493,7 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17" t="s">
@@ -12506,7 +12507,7 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17" t="s">
@@ -12520,7 +12521,7 @@
       </c>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17" t="s">
@@ -12534,7 +12535,7 @@
       </c>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17" t="s">
@@ -12550,7 +12551,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17" t="s">
@@ -12564,7 +12565,7 @@
       </c>
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17" t="s">
@@ -12989,14 +12990,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="F123" sqref="F123:F124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
@@ -13027,21 +13028,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="29.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>611</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>612</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>613</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+    </row>
+    <row r="3" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -13049,7 +13050,7 @@
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="17"/>
       <c r="B4" s="17" t="s">
         <v>614</v>
@@ -13065,7 +13066,7 @@
       </c>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17" t="s">
@@ -13079,7 +13080,7 @@
       </c>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17" t="s">
@@ -13093,7 +13094,7 @@
       </c>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
@@ -13101,7 +13102,7 @@
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
       <c r="B8" s="17" t="s">
         <v>621</v>
@@ -13117,7 +13118,7 @@
       </c>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17" t="s">
@@ -13131,7 +13132,7 @@
       </c>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17" t="s">
@@ -13145,7 +13146,7 @@
       </c>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -13153,7 +13154,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17" t="s">
@@ -13167,7 +13168,7 @@
       </c>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17" t="s">
@@ -13181,7 +13182,7 @@
       </c>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17" t="s">
@@ -13195,7 +13196,7 @@
       </c>
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="17"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17" t="s">
@@ -13209,7 +13210,7 @@
       </c>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17" t="s">
@@ -13223,7 +13224,7 @@
       </c>
       <c r="F16" s="17"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="17"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17" t="s">
@@ -13237,7 +13238,7 @@
       </c>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17" t="s">
@@ -13919,7 +13920,7 @@
       </c>
       <c r="F70" s="17"/>
     </row>
-    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="17" t="s">
@@ -13963,7 +13964,7 @@
       </c>
       <c r="F73" s="17"/>
     </row>
-    <row r="74" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="17" t="s">
@@ -13990,7 +13991,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="17" t="s">
@@ -14017,7 +14018,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="17"/>
       <c r="B78" s="17"/>
       <c r="C78" s="17" t="s">
@@ -14045,7 +14046,7 @@
       </c>
       <c r="F79" s="17"/>
     </row>
-    <row r="80" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="17"/>
       <c r="B80" s="17"/>
       <c r="C80" s="17" t="s">
@@ -14107,7 +14108,7 @@
       </c>
       <c r="F84" s="17"/>
     </row>
-    <row r="85" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A85" s="17"/>
       <c r="B85" s="17"/>
       <c r="C85" s="17" t="s">
@@ -14175,7 +14176,7 @@
       </c>
       <c r="F89" s="17"/>
     </row>
-    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A90" s="17"/>
       <c r="B90" s="17"/>
       <c r="C90" s="17" t="s">
@@ -14465,7 +14466,7 @@
       </c>
       <c r="F110" s="17"/>
     </row>
-    <row r="111" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A111" s="17"/>
       <c r="B111" s="17"/>
       <c r="C111" s="17" t="s">
@@ -14479,7 +14480,7 @@
       </c>
       <c r="F111" s="17"/>
     </row>
-    <row r="112" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="15.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="17"/>
       <c r="B112" s="17"/>
       <c r="C112" s="17" t="s">
@@ -14506,7 +14507,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" ht="17.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="17"/>
       <c r="B114" s="17"/>
       <c r="C114" s="17" t="s">
@@ -14520,7 +14521,7 @@
       </c>
       <c r="F114" s="17"/>
     </row>
-    <row r="115" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A115" s="17"/>
       <c r="B115" s="17"/>
       <c r="C115" s="17" t="s">
@@ -14548,7 +14549,7 @@
       </c>
       <c r="F116" s="17"/>
     </row>
-    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="17"/>
       <c r="B117" s="17"/>
       <c r="C117" s="17" t="s">
@@ -14590,7 +14591,7 @@
       </c>
       <c r="F119" s="17"/>
     </row>
-    <row r="120" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="17"/>
       <c r="B120" s="17"/>
       <c r="C120" s="17" t="s">
@@ -14626,9 +14627,11 @@
       <c r="E122" s="17"/>
       <c r="F122" s="17"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="17"/>
-      <c r="B123" s="17"/>
+      <c r="B123" s="17" t="s">
+        <v>1322</v>
+      </c>
       <c r="C123" s="17" t="s">
         <v>828</v>
       </c>
@@ -14638,7 +14641,9 @@
       <c r="E123" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="F123" s="17"/>
+      <c r="F123" s="29" t="s">
+        <v>1323</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="17"/>
@@ -14652,7 +14657,7 @@
       <c r="E124" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="F124" s="17"/>
+      <c r="F124" s="29"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="17"/>
@@ -14679,14 +14684,24 @@
       <c r="F126" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C2:F2"/>
+    <mergeCell ref="F123:F124"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -14736,9 +14751,9 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="478" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="530d37be357ae9af341f1311dafd44e2">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f1b0c369e886228bd2ebc7f10ef132e9" ns1:_="" ns2:_="" ns3:_="">
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="480" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4112082b3fcc37184355d8d9f746cc16">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e31d9155d0f1567779179698607192e" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
     <xsd:import namespace="d16efad5-0601-4cf0-b7c2-89968258c777"/>
@@ -14764,6 +14779,8 @@
                 <xsd:element ref="ns2:Survey_x0020_Type" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -14837,6 +14854,18 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="24" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="25" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="26" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -14991,7 +15020,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -15006,16 +15035,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90E9E434-4B8B-4BAE-8E0F-2B34F42316A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C070FFD4-2B81-40A9-9526-59DD893E6C18}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -15023,8 +15051,8 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50E825E5-D295-4ACF-B8F3-CD5493E2774D}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{096B1B8F-85B6-4F7D-B099-9F3595B615B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -15043,7 +15071,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC59F560-844B-432B-8AD6-73714CEDFB96}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -15059,12 +15087,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90E9E434-4B8B-4BAE-8E0F-2B34F42316A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Chapters 3 and 15 completed
Chapter 3 - Respondents' Characteristics and Chapter 15 - Women's Empowerment are complete.
</commit_message>
<xml_diff>
--- a/IndicatorList.xlsx
+++ b/IndicatorList.xlsx
@@ -11711,8 +11711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Chapter 11 - Nutrition
Code available for the nutrition chapter - chapter 11
</commit_message>
<xml_diff>
--- a/IndicatorList.xlsx
+++ b/IndicatorList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33697\ICF\Analysis - Shared Resources\Code\DHS-Indicators-Stata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="194" documentId="114_{BA56B5EA-75AF-4E8A-BCB2-6B6346BBE5CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{79AEAB84-472F-4213-A918-0BF403EA1E9D}"/>
+  <xr:revisionPtr revIDLastSave="465" documentId="114_{BA56B5EA-75AF-4E8A-BCB2-6B6346BBE5CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{7B4D877E-4772-44E9-9B2A-04D72CB226AD}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" tabRatio="690" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1139" yWindow="1139" windowWidth="18851" windowHeight="11808" tabRatio="690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH2PH" sheetId="17" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2503" uniqueCount="1690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="1849">
   <si>
     <t>Chapter</t>
   </si>
@@ -5116,6 +5116,483 @@
   </si>
   <si>
     <t>nt_mn_bmi_mean</t>
+  </si>
+  <si>
+    <t>Population and Housing</t>
+  </si>
+  <si>
+    <t>PHmaster.do</t>
+  </si>
+  <si>
+    <t>Master file for the Population and Housing chapter. The master file will call the do file listed below and the PH_tables.do file not listed here. The tables do file will produce excel tables of the indicators.</t>
+  </si>
+  <si>
+    <t>PH_WATER.do</t>
+  </si>
+  <si>
+    <t>HR or PR</t>
+  </si>
+  <si>
+    <t>"Source of drinking water"</t>
+  </si>
+  <si>
+    <t>"Access to improved water source"</t>
+  </si>
+  <si>
+    <t>"Round trip time to obtain drinking water"</t>
+  </si>
+  <si>
+    <t>ph_wtr_source</t>
+  </si>
+  <si>
+    <t>ph_wtr_improved</t>
+  </si>
+  <si>
+    <t>ph_wtr_time</t>
+  </si>
+  <si>
+    <t>ph_wtr_treat_boil</t>
+  </si>
+  <si>
+    <t>"Treated water by boiling before drinking"</t>
+  </si>
+  <si>
+    <t>ph_wtr_treat_clth</t>
+  </si>
+  <si>
+    <t>ph_wtr_treat_chlr</t>
+  </si>
+  <si>
+    <t>ph_wtr_treat_fltr</t>
+  </si>
+  <si>
+    <t>ph_wtr_treat_solr</t>
+  </si>
+  <si>
+    <t>ph_wtr_treat_stnd</t>
+  </si>
+  <si>
+    <t>ph_wtr_treat_othr</t>
+  </si>
+  <si>
+    <t>ph_wtr_no_treat</t>
+  </si>
+  <si>
+    <t>"Treated water by adding bleach or chlorine before drinking"</t>
+  </si>
+  <si>
+    <t>"Treated water by straining through cloth before drinking"</t>
+  </si>
+  <si>
+    <t>"Treated water by ceramic, sand, or other filter before drinking"</t>
+  </si>
+  <si>
+    <t>"Treated water by solar disinfection before drinking"</t>
+  </si>
+  <si>
+    <t>"Treated water by letting stand and settle before drinking"</t>
+  </si>
+  <si>
+    <t>"Treated water by other means before drinking"</t>
+  </si>
+  <si>
+    <t>"Did not treat water before drinking"</t>
+  </si>
+  <si>
+    <t>ph_wtr_avail</t>
+  </si>
+  <si>
+    <t>"Availability of water among those using piped water or water from tube well or borehole"</t>
+  </si>
+  <si>
+    <t>PH_SANIT.do</t>
+  </si>
+  <si>
+    <t>ph_sanit_type</t>
+  </si>
+  <si>
+    <t>"Type of sanitation facility"</t>
+  </si>
+  <si>
+    <t>ph_sanit_improved</t>
+  </si>
+  <si>
+    <t>"Access to improved sanitation"</t>
+  </si>
+  <si>
+    <t>ph_sanit_location</t>
+  </si>
+  <si>
+    <t>"Location of toilet/latrine facility"</t>
+  </si>
+  <si>
+    <t>PH_HOUS.do</t>
+  </si>
+  <si>
+    <t>ph_electric</t>
+  </si>
+  <si>
+    <t>"Have electricity"</t>
+  </si>
+  <si>
+    <t>ph_floor</t>
+  </si>
+  <si>
+    <t>"Flooring material"</t>
+  </si>
+  <si>
+    <t>ph_rooms_sleep</t>
+  </si>
+  <si>
+    <t>"Rooms for sleeping"</t>
+  </si>
+  <si>
+    <t>"Place for cooking"</t>
+  </si>
+  <si>
+    <t>ph_cook_place</t>
+  </si>
+  <si>
+    <t>ph_cook_fuel</t>
+  </si>
+  <si>
+    <t>"Type fo cooking fuel"</t>
+  </si>
+  <si>
+    <t>ph_cook_solid</t>
+  </si>
+  <si>
+    <t>"Using solid fuel for cooking"</t>
+  </si>
+  <si>
+    <t>ph_cook_clean</t>
+  </si>
+  <si>
+    <t>"Using clean fuel for cooking"</t>
+  </si>
+  <si>
+    <t>ph_smoke</t>
+  </si>
+  <si>
+    <t>"Frequency of smoking at home"</t>
+  </si>
+  <si>
+    <t>ph_radio</t>
+  </si>
+  <si>
+    <t>ph_tv</t>
+  </si>
+  <si>
+    <t>ph_mobile</t>
+  </si>
+  <si>
+    <t>ph_tel</t>
+  </si>
+  <si>
+    <t>ph_comp</t>
+  </si>
+  <si>
+    <t>ph_frig</t>
+  </si>
+  <si>
+    <t>ph_bike</t>
+  </si>
+  <si>
+    <t>ph_cart</t>
+  </si>
+  <si>
+    <t>ph_moto</t>
+  </si>
+  <si>
+    <t>ph_car</t>
+  </si>
+  <si>
+    <t>ph_boat</t>
+  </si>
+  <si>
+    <t>ph_agriland</t>
+  </si>
+  <si>
+    <t>ph_animals</t>
+  </si>
+  <si>
+    <t>"Owns a radio"</t>
+  </si>
+  <si>
+    <t>"Owns a tv"</t>
+  </si>
+  <si>
+    <t>"Owns a non-mobile telephone"</t>
+  </si>
+  <si>
+    <t>"Owns a mobile phone"</t>
+  </si>
+  <si>
+    <t>"Owns a computer"</t>
+  </si>
+  <si>
+    <t>"Owns a refrigerator"</t>
+  </si>
+  <si>
+    <t>"Owns a bicycle"</t>
+  </si>
+  <si>
+    <t>"Owns a motorcycle/scooter"</t>
+  </si>
+  <si>
+    <t>"Owns a car or truck"</t>
+  </si>
+  <si>
+    <t>"Owns a boat with a motor"</t>
+  </si>
+  <si>
+    <t>"Owns agricultural land"</t>
+  </si>
+  <si>
+    <t>"Owns livestock or farm animals"</t>
+  </si>
+  <si>
+    <t>ph_wealth_quint</t>
+  </si>
+  <si>
+    <t>"Wealth quintile"</t>
+  </si>
+  <si>
+    <t>ph_wealth_gini</t>
+  </si>
+  <si>
+    <t>"Gini coefficient of wealth index"</t>
+  </si>
+  <si>
+    <t>PH_HNDWSH.do</t>
+  </si>
+  <si>
+    <t>"Fixed place for handwashing"</t>
+  </si>
+  <si>
+    <t>"Mobile place for handwashing"</t>
+  </si>
+  <si>
+    <t>"Either fixed or mobile place for handwashing"</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_plac_both</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_place_mob</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_place_fxd</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_wtronly</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_soap_nowtr</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_soap_wtr</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_clnsagnt_wtr</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_clnsagnt_nowtr</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_none</t>
+  </si>
+  <si>
+    <t>"Place observed for handwashing with soap and water"</t>
+  </si>
+  <si>
+    <t>"Place observed for handwashing with cleansing agent other than soap and water"</t>
+  </si>
+  <si>
+    <t>"Place observed for handwashing with water only"</t>
+  </si>
+  <si>
+    <t>"Place observed for handwashing with soap and no water"</t>
+  </si>
+  <si>
+    <t>"Place observed for handwashing with cleansing agent otherthan soap and no water"</t>
+  </si>
+  <si>
+    <t>"Place observed for handwashing with no water, no soap, and no other cleansing agent"</t>
+  </si>
+  <si>
+    <t>PH_POP.do</t>
+  </si>
+  <si>
+    <t>ph_pop_age</t>
+  </si>
+  <si>
+    <t>ph_pop_depend</t>
+  </si>
+  <si>
+    <t>ph_pop_cld_adlt</t>
+  </si>
+  <si>
+    <t>ph_pop_adols</t>
+  </si>
+  <si>
+    <t>"De facto population by five-year age groups"</t>
+  </si>
+  <si>
+    <t>"De facto population by dependency age groups"</t>
+  </si>
+  <si>
+    <t>"De facto population by child and adult populations"</t>
+  </si>
+  <si>
+    <t>"De factor population that are adolesents"</t>
+  </si>
+  <si>
+    <t>ph_hhhead_sex</t>
+  </si>
+  <si>
+    <t>"Sex of household head"</t>
+  </si>
+  <si>
+    <t>ph_num_members</t>
+  </si>
+  <si>
+    <t>"Number of usual household members"</t>
+  </si>
+  <si>
+    <t>ph_mean_hhsize</t>
+  </si>
+  <si>
+    <t>"Mean size of household"</t>
+  </si>
+  <si>
+    <t>ph_orph_double</t>
+  </si>
+  <si>
+    <t>ph_orph_single</t>
+  </si>
+  <si>
+    <t>ph_orph_foster</t>
+  </si>
+  <si>
+    <t>ph_foster</t>
+  </si>
+  <si>
+    <t>"Double orphans under age 18"</t>
+  </si>
+  <si>
+    <t>"Single orphans under age 18"</t>
+  </si>
+  <si>
+    <t>"Foster children under age 18"</t>
+  </si>
+  <si>
+    <t>"Orphans and/or foster children under age 18"</t>
+  </si>
+  <si>
+    <t>HR and PR</t>
+  </si>
+  <si>
+    <t>"Child under 18 not living with a biological parent"</t>
+  </si>
+  <si>
+    <t>ph_birthreg_cert</t>
+  </si>
+  <si>
+    <t>"Child under 5 with registered birth and birth certificate"</t>
+  </si>
+  <si>
+    <t>ph_birthreg_nocert</t>
+  </si>
+  <si>
+    <t>"Child under 5 with registered birth"</t>
+  </si>
+  <si>
+    <t>ph_birthreg</t>
+  </si>
+  <si>
+    <t>PH_EDU.do</t>
+  </si>
+  <si>
+    <t>ph_highest_edu</t>
+  </si>
+  <si>
+    <t>ph_median_eduyrs</t>
+  </si>
+  <si>
+    <t>"Highest level of schooling attended or completed among those age 6 or over"</t>
+  </si>
+  <si>
+    <t>"Median years of education among those age 6 or over"</t>
+  </si>
+  <si>
+    <t>"Primary school net attendance ratio (NAR)"</t>
+  </si>
+  <si>
+    <t>"Secondary school net attendance ratio (NAR)"</t>
+  </si>
+  <si>
+    <t>ph_sch_nar_prim</t>
+  </si>
+  <si>
+    <t>ph_sch_nar_sec</t>
+  </si>
+  <si>
+    <t>ph_sch_gar_prim</t>
+  </si>
+  <si>
+    <t>ph_sch_gar_sec</t>
+  </si>
+  <si>
+    <t>ph_gpi_nar_prim</t>
+  </si>
+  <si>
+    <t>ph_gpi_nar_sec</t>
+  </si>
+  <si>
+    <t>ph_gpi_gar_prim</t>
+  </si>
+  <si>
+    <t>ph_gpi_gar_sec</t>
+  </si>
+  <si>
+    <t>"Primary school gross attendance ratio (GAR)"</t>
+  </si>
+  <si>
+    <t>"Secondary school gross attendance ratio (GAR)"</t>
+  </si>
+  <si>
+    <t>"Gender parity index for NAR primary"</t>
+  </si>
+  <si>
+    <t>"Gender parity index for GAR primary"</t>
+  </si>
+  <si>
+    <t>"Gender parity index for NAR secondary"</t>
+  </si>
+  <si>
+    <t>"Gender parity index for GAR secondary"</t>
+  </si>
+  <si>
+    <t>"Owns a animal drawn cart"</t>
+  </si>
+  <si>
+    <t>ph_chld_liv_arrang</t>
+  </si>
+  <si>
+    <t>ph_chld_liv_noprnt</t>
+  </si>
+  <si>
+    <t>ph_chld_orph</t>
+  </si>
+  <si>
+    <t>"Child under 18 with one or both parents dead"</t>
+  </si>
+  <si>
+    <t>"Child under 5 with registered birth and no birth certificate"</t>
+  </si>
+  <si>
+    <t>"Living arrangement and parents survival status for child under 18"</t>
   </si>
 </sst>
 </file>
@@ -5246,7 +5723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5378,6 +5855,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -5685,14 +6174,1065 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="70.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.44140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>1692</v>
+      </c>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="50"/>
+      <c r="B4" s="50" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>1698</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>1695</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F4" s="50"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50" t="s">
+        <v>1699</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>1696</v>
+      </c>
+      <c r="E5" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F5" s="50"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="50"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50" t="s">
+        <v>1700</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>1697</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F6" s="50"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50" t="s">
+        <v>1701</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>1702</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F7" s="50"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>1710</v>
+      </c>
+      <c r="E8" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F8" s="50"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50" t="s">
+        <v>1703</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>1711</v>
+      </c>
+      <c r="E9" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F9" s="50"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50" t="s">
+        <v>1705</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>1712</v>
+      </c>
+      <c r="E10" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F10" s="50"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="50"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50" t="s">
+        <v>1706</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F11" s="50"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50" t="s">
+        <v>1707</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>1714</v>
+      </c>
+      <c r="E12" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F12" s="50"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="50"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50" t="s">
+        <v>1708</v>
+      </c>
+      <c r="D13" s="50" t="s">
+        <v>1715</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F13" s="50"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50" t="s">
+        <v>1709</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F14" s="50"/>
+    </row>
+    <row r="15" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="A15" s="50"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50" t="s">
+        <v>1717</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>1718</v>
+      </c>
+      <c r="E15" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F15" s="50"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="50"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="50"/>
+      <c r="B17" s="50" t="s">
+        <v>1719</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>1720</v>
+      </c>
+      <c r="D17" s="50" t="s">
+        <v>1721</v>
+      </c>
+      <c r="E17" s="50" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F17" s="50"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="50"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50" t="s">
+        <v>1722</v>
+      </c>
+      <c r="D18" s="52" t="s">
+        <v>1723</v>
+      </c>
+      <c r="E18" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F18" s="50"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="50"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50" t="s">
+        <v>1724</v>
+      </c>
+      <c r="D19" s="50" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E19" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F19" s="50"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="50"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="50"/>
+      <c r="B21" s="50" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>1727</v>
+      </c>
+      <c r="D21" s="50" t="s">
+        <v>1728</v>
+      </c>
+      <c r="E21" s="50" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F21" s="50"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="50"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50" t="s">
+        <v>1729</v>
+      </c>
+      <c r="D22" s="50" t="s">
+        <v>1730</v>
+      </c>
+      <c r="E22" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F22" s="50"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="50"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50" t="s">
+        <v>1731</v>
+      </c>
+      <c r="D23" s="50" t="s">
+        <v>1732</v>
+      </c>
+      <c r="E23" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F23" s="50"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="50"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50" t="s">
+        <v>1734</v>
+      </c>
+      <c r="D24" s="50" t="s">
+        <v>1733</v>
+      </c>
+      <c r="E24" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F24" s="50"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="50"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50" t="s">
+        <v>1735</v>
+      </c>
+      <c r="D25" s="50" t="s">
+        <v>1736</v>
+      </c>
+      <c r="E25" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F25" s="50"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="50"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50" t="s">
+        <v>1737</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>1738</v>
+      </c>
+      <c r="E26" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F26" s="50"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="50"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50" t="s">
+        <v>1739</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>1740</v>
+      </c>
+      <c r="E27" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F27" s="50"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="52"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="52"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="52" t="s">
+        <v>1743</v>
+      </c>
+      <c r="D29" s="52" t="s">
+        <v>1756</v>
+      </c>
+      <c r="E29" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F29" s="52"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="52"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52" t="s">
+        <v>1744</v>
+      </c>
+      <c r="D30" s="52" t="s">
+        <v>1757</v>
+      </c>
+      <c r="E30" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F30" s="52"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="52"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52" t="s">
+        <v>1745</v>
+      </c>
+      <c r="D31" s="52" t="s">
+        <v>1759</v>
+      </c>
+      <c r="E31" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F31" s="52"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="52"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52" t="s">
+        <v>1746</v>
+      </c>
+      <c r="D32" s="52" t="s">
+        <v>1758</v>
+      </c>
+      <c r="E32" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F32" s="52"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="52"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="52" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D33" s="52" t="s">
+        <v>1760</v>
+      </c>
+      <c r="E33" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F33" s="52"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="50"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="50" t="s">
+        <v>1748</v>
+      </c>
+      <c r="D34" s="52" t="s">
+        <v>1761</v>
+      </c>
+      <c r="E34" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F34" s="50"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="52"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="52" t="s">
+        <v>1749</v>
+      </c>
+      <c r="D35" s="52" t="s">
+        <v>1762</v>
+      </c>
+      <c r="E35" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F35" s="52"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="52"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52" t="s">
+        <v>1750</v>
+      </c>
+      <c r="D36" s="52" t="s">
+        <v>1842</v>
+      </c>
+      <c r="E36" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F36" s="52"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="52"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="52" t="s">
+        <v>1751</v>
+      </c>
+      <c r="D37" s="52" t="s">
+        <v>1763</v>
+      </c>
+      <c r="E37" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F37" s="52"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="52"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="52" t="s">
+        <v>1752</v>
+      </c>
+      <c r="D38" s="52" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E38" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F38" s="52"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="52"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="52" t="s">
+        <v>1753</v>
+      </c>
+      <c r="D39" s="52" t="s">
+        <v>1765</v>
+      </c>
+      <c r="E39" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F39" s="52"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="52"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="52" t="s">
+        <v>1754</v>
+      </c>
+      <c r="D40" s="52" t="s">
+        <v>1766</v>
+      </c>
+      <c r="E40" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F40" s="52"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="52"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="52" t="s">
+        <v>1755</v>
+      </c>
+      <c r="D41" s="52" t="s">
+        <v>1767</v>
+      </c>
+      <c r="E41" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F41" s="52"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="52"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="50"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50" t="s">
+        <v>1741</v>
+      </c>
+      <c r="D43" s="50" t="s">
+        <v>1742</v>
+      </c>
+      <c r="E43" s="50" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F43" s="50"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="50"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="50"/>
+      <c r="B45" s="50" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C45" s="50" t="s">
+        <v>1778</v>
+      </c>
+      <c r="D45" s="50" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E45" s="50" t="s">
+        <v>871</v>
+      </c>
+      <c r="F45" s="50"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="50"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D46" s="50" t="s">
+        <v>1774</v>
+      </c>
+      <c r="E46" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F46" s="50"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="50"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50" t="s">
+        <v>1776</v>
+      </c>
+      <c r="D47" s="50" t="s">
+        <v>1775</v>
+      </c>
+      <c r="E47" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F47" s="50"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="50"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="50" t="s">
+        <v>1781</v>
+      </c>
+      <c r="D48" s="50" t="s">
+        <v>1785</v>
+      </c>
+      <c r="E48" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F48" s="50"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="50"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="50" t="s">
+        <v>1782</v>
+      </c>
+      <c r="D49" s="52" t="s">
+        <v>1786</v>
+      </c>
+      <c r="E49" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F49" s="50"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C50" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="D50" s="52" t="s">
+        <v>1787</v>
+      </c>
+      <c r="E50" s="52" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C51" s="1" t="s">
+        <v>1780</v>
+      </c>
+      <c r="D51" s="52" t="s">
+        <v>1788</v>
+      </c>
+      <c r="E51" s="52" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C52" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="D52" s="52" t="s">
+        <v>1789</v>
+      </c>
+      <c r="E52" s="52" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="1" t="s">
+        <v>1784</v>
+      </c>
+      <c r="D53" s="52" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E53" s="52" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B55" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>1792</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>1796</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C56" s="1" t="s">
+        <v>1793</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>1797</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C57" s="1" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>1798</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C58" s="1" t="s">
+        <v>1795</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>1799</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C59" s="1" t="s">
+        <v>1800</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C60" s="1" t="s">
+        <v>1802</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C61" s="1" t="s">
+        <v>1804</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="52"/>
+      <c r="B63" s="52"/>
+      <c r="C63" s="52" t="s">
+        <v>1768</v>
+      </c>
+      <c r="D63" s="52" t="s">
+        <v>1769</v>
+      </c>
+      <c r="E63" s="52" t="s">
+        <v>851</v>
+      </c>
+      <c r="F63" s="52"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="52"/>
+      <c r="B64" s="52"/>
+      <c r="C64" s="52" t="s">
+        <v>1770</v>
+      </c>
+      <c r="D64" s="52" t="s">
+        <v>1771</v>
+      </c>
+      <c r="E64" s="52" t="s">
+        <v>851</v>
+      </c>
+      <c r="F64" s="52"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="53"/>
+      <c r="B65" s="53"/>
+      <c r="C65" s="53"/>
+      <c r="D65" s="53"/>
+      <c r="E65" s="53"/>
+      <c r="F65" s="53"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C66" s="1" t="s">
+        <v>1806</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>1810</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C67" s="1" t="s">
+        <v>1807</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>1811</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C68" s="1" t="s">
+        <v>1809</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>1812</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C69" s="1" t="s">
+        <v>1808</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>1813</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C71" s="1" t="s">
+        <v>1843</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>1848</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C72" s="1" t="s">
+        <v>1844</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C73" s="1" t="s">
+        <v>1845</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>1846</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C75" s="1" t="s">
+        <v>1816</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C76" s="1" t="s">
+        <v>1818</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>1847</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C77" s="1" t="s">
+        <v>1820</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B79" s="1" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>1822</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>1824</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C80" s="1" t="s">
+        <v>1823</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C82" s="1" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>1826</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C83" s="1" t="s">
+        <v>1829</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>1827</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="84" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C84" s="1" t="s">
+        <v>1830</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C85" s="1" t="s">
+        <v>1831</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>1837</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C86" s="1" t="s">
+        <v>1832</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C87" s="1" t="s">
+        <v>1833</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>1840</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="88" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C88" s="1" t="s">
+        <v>1834</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>1839</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="89" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C89" s="1" t="s">
+        <v>1835</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>1841</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5701,7 +7241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -5743,12 +7283,12 @@
       <c r="B2" s="17" t="s">
         <v>808</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="57" t="s">
         <v>809</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
     </row>
     <row r="3" spans="1:6" ht="15.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -7243,12 +8783,12 @@
       <c r="B2" s="17" t="s">
         <v>875</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="57" t="s">
         <v>876</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
     </row>
     <row r="3" spans="1:6" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
@@ -7446,7 +8986,7 @@
       <c r="E16" s="17" t="s">
         <v>910</v>
       </c>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="59" t="s">
         <v>911</v>
       </c>
     </row>
@@ -7460,7 +9000,7 @@
         <v>913</v>
       </c>
       <c r="E17" s="17"/>
-      <c r="F17" s="55"/>
+      <c r="F17" s="59"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
@@ -7536,7 +9076,7 @@
       <c r="E23" s="17" t="s">
         <v>851</v>
       </c>
-      <c r="F23" s="56" t="s">
+      <c r="F23" s="60" t="s">
         <v>925</v>
       </c>
     </row>
@@ -7552,7 +9092,7 @@
       <c r="E24" s="17" t="s">
         <v>851</v>
       </c>
-      <c r="F24" s="56"/>
+      <c r="F24" s="60"/>
     </row>
     <row r="25" spans="1:6" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
@@ -7566,7 +9106,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="54" t="s">
         <v>929</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -7584,7 +9124,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="17"/>
-      <c r="B27" s="50"/>
+      <c r="B27" s="54"/>
       <c r="C27" s="1" t="s">
         <v>933</v>
       </c>
@@ -7600,7 +9140,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
-      <c r="B28" s="50"/>
+      <c r="B28" s="54"/>
       <c r="C28" s="1" t="s">
         <v>935</v>
       </c>
@@ -7616,7 +9156,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
-      <c r="B29" s="50"/>
+      <c r="B29" s="54"/>
       <c r="C29" s="17" t="s">
         <v>937</v>
       </c>
@@ -7630,7 +9170,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
-      <c r="B30" s="50"/>
+      <c r="B30" s="54"/>
       <c r="C30" s="17" t="s">
         <v>939</v>
       </c>
@@ -7644,7 +9184,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
-      <c r="B31" s="50"/>
+      <c r="B31" s="54"/>
       <c r="C31" s="17" t="s">
         <v>941</v>
       </c>
@@ -8256,12 +9796,12 @@
       <c r="B2" s="21" t="s">
         <v>1004</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="57" t="s">
         <v>1005</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
     </row>
     <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F3" s="22"/>
@@ -8502,7 +10042,7 @@
       <c r="E26" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="57" t="s">
+      <c r="F26" s="61" t="s">
         <v>1025</v>
       </c>
       <c r="G26" s="34"/>
@@ -8517,7 +10057,7 @@
       <c r="E27" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="57"/>
+      <c r="F27" s="61"/>
     </row>
     <row r="28" spans="2:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="24" t="s">
@@ -8529,7 +10069,7 @@
       <c r="E28" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="57"/>
+      <c r="F28" s="61"/>
       <c r="G28" s="34"/>
     </row>
     <row r="29" spans="2:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
@@ -8542,7 +10082,7 @@
       <c r="E29" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="57"/>
+      <c r="F29" s="61"/>
     </row>
     <row r="30" spans="2:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24" t="s">
@@ -9043,12 +10583,12 @@
       <c r="B2" s="21" t="s">
         <v>1064</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="57" t="s">
         <v>1094</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="s">
@@ -9091,7 +10631,7 @@
       <c r="E7" s="24" t="s">
         <v>1072</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="61" t="s">
         <v>1073</v>
       </c>
     </row>
@@ -9105,7 +10645,7 @@
       <c r="E8" s="24" t="s">
         <v>1072</v>
       </c>
-      <c r="F8" s="57"/>
+      <c r="F8" s="61"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" s="24" t="s">
@@ -9117,7 +10657,7 @@
       <c r="E9" s="24" t="s">
         <v>1072</v>
       </c>
-      <c r="F9" s="57"/>
+      <c r="F9" s="61"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F10" s="42"/>
@@ -9363,12 +10903,12 @@
       <c r="B2" s="21" t="s">
         <v>1093</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="57" t="s">
         <v>1095</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -9805,12 +11345,12 @@
       <c r="B2" s="26" t="s">
         <v>1210</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="57" t="s">
         <v>1209</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -10690,7 +12230,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -10731,12 +12271,12 @@
       <c r="B2" s="4" t="s">
         <v>1111</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="54" t="s">
         <v>1112</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
@@ -11285,12 +12825,12 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
@@ -11675,12 +13215,12 @@
       <c r="B2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -12489,12 +14029,12 @@
       <c r="B2" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -12688,12 +14228,12 @@
       <c r="B2" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="57" t="s">
         <v>145</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
@@ -13063,7 +14603,7 @@
       <c r="E29" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="53" t="s">
+      <c r="F29" s="57" t="s">
         <v>199</v>
       </c>
     </row>
@@ -13079,7 +14619,7 @@
       <c r="E30" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="53"/>
+      <c r="F30" s="57"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
@@ -13093,7 +14633,7 @@
       <c r="E31" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="53"/>
+      <c r="F31" s="57"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
@@ -13107,7 +14647,7 @@
       <c r="E32" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="57"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
@@ -13121,7 +14661,7 @@
       <c r="E33" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="53"/>
+      <c r="F33" s="57"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="17"/>
@@ -13135,7 +14675,7 @@
       <c r="E34" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="53"/>
+      <c r="F34" s="57"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
@@ -13149,7 +14689,7 @@
       <c r="E35" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="53"/>
+      <c r="F35" s="57"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="17"/>
@@ -13163,7 +14703,7 @@
       <c r="E36" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="53"/>
+      <c r="F36" s="57"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="17"/>
@@ -13177,7 +14717,7 @@
       <c r="E37" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="53"/>
+      <c r="F37" s="57"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="17"/>
@@ -13191,7 +14731,7 @@
       <c r="E38" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="53"/>
+      <c r="F38" s="57"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="17"/>
@@ -13205,7 +14745,7 @@
       <c r="E39" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="53"/>
+      <c r="F39" s="57"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="17"/>
@@ -13219,7 +14759,7 @@
       <c r="E40" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="53"/>
+      <c r="F40" s="57"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="17"/>
@@ -13233,7 +14773,7 @@
       <c r="E41" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F41" s="53"/>
+      <c r="F41" s="57"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="17"/>
@@ -13247,7 +14787,7 @@
       <c r="E42" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F42" s="53"/>
+      <c r="F42" s="57"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="17"/>
@@ -13261,7 +14801,7 @@
       <c r="E43" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="53"/>
+      <c r="F43" s="57"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="17"/>
@@ -13275,7 +14815,7 @@
       <c r="E44" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="53"/>
+      <c r="F44" s="57"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="17"/>
@@ -13289,7 +14829,7 @@
       <c r="E45" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F45" s="53"/>
+      <c r="F45" s="57"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="17"/>
@@ -13303,7 +14843,7 @@
       <c r="E46" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F46" s="53"/>
+      <c r="F46" s="57"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="17"/>
@@ -13835,7 +15375,7 @@
       <c r="E86" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F86" s="53" t="s">
+      <c r="F86" s="57" t="s">
         <v>305</v>
       </c>
     </row>
@@ -13851,7 +15391,7 @@
       <c r="E87" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F87" s="53"/>
+      <c r="F87" s="57"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="17"/>
@@ -13865,7 +15405,7 @@
       <c r="E88" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F88" s="53"/>
+      <c r="F88" s="57"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="17"/>
@@ -13879,7 +15419,7 @@
       <c r="E89" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F89" s="53"/>
+      <c r="F89" s="57"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="17"/>
@@ -13893,7 +15433,7 @@
       <c r="E90" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F90" s="53"/>
+      <c r="F90" s="57"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="17"/>
@@ -13907,7 +15447,7 @@
       <c r="E91" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F91" s="53"/>
+      <c r="F91" s="57"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="17"/>
@@ -13921,7 +15461,7 @@
       <c r="E92" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F92" s="53"/>
+      <c r="F92" s="57"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="17"/>
@@ -13935,7 +15475,7 @@
       <c r="E93" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F93" s="53"/>
+      <c r="F93" s="57"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="17"/>
@@ -13949,7 +15489,7 @@
       <c r="E94" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F94" s="53"/>
+      <c r="F94" s="57"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="17"/>
@@ -13963,7 +15503,7 @@
       <c r="E95" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F95" s="53"/>
+      <c r="F95" s="57"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="17"/>
@@ -13977,7 +15517,7 @@
       <c r="E96" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F96" s="53"/>
+      <c r="F96" s="57"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="17"/>
@@ -13991,7 +15531,7 @@
       <c r="E97" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F97" s="53"/>
+      <c r="F97" s="57"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="17"/>
@@ -14005,7 +15545,7 @@
       <c r="E98" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F98" s="53"/>
+      <c r="F98" s="57"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="17"/>
@@ -14019,7 +15559,7 @@
       <c r="E99" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F99" s="53"/>
+      <c r="F99" s="57"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="17"/>
@@ -14694,12 +16234,12 @@
       <c r="B2" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="56" t="s">
         <v>417</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -14714,10 +16254,10 @@
       <c r="B4" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="58" t="s">
         <v>419</v>
       </c>
-      <c r="D4" s="54"/>
+      <c r="D4" s="58"/>
       <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
@@ -15456,12 +16996,12 @@
       <c r="B2" s="17" t="s">
         <v>501</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="57" t="s">
         <v>502</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
@@ -16099,12 +17639,12 @@
       <c r="B2" s="17" t="s">
         <v>585</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="57" t="s">
         <v>586</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
@@ -17705,7 +19245,7 @@
       <c r="E123" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="F123" s="53" t="s">
+      <c r="F123" s="57" t="s">
         <v>1097</v>
       </c>
     </row>
@@ -17721,7 +19261,7 @@
       <c r="E124" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="F124" s="53"/>
+      <c r="F124" s="57"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="17"/>
@@ -17772,6 +19312,65 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="481" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be21cae339529f0f311ef097f4a87693">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd9e5a0c56088652e9b5d1a36fcd7f8a" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -18040,65 +19639,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC59F560-844B-432B-8AD6-73714CEDFB96}">
   <ds:schemaRefs>
@@ -18118,6 +19658,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90E9E434-4B8B-4BAE-8E0F-2B34F42316A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C070FFD4-2B81-40A9-9526-59DD893E6C18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C215EABC-DB34-46B5-A5E5-21478E186E0D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18135,20 +19691,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C070FFD4-2B81-40A9-9526-59DD893E6C18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90E9E434-4B8B-4BAE-8E0F-2B34F42316A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Upload of Chapter 19 - Fistula
Please read the notes in the do file. The variables for this chapter are not standardized and will be different from one survey to the next. You need to find the correct variables according to the variable lables as described in the notes.
</commit_message>
<xml_diff>
--- a/IndicatorList.xlsx
+++ b/IndicatorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33697\ICF\Analysis - Shared Resources\Code\DHS-Indicators-Stata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/Shared Resources/Code/DHS-Indicators-Stata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB928E38-4282-43C6-806C-7944B958E23F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="114_{17F82F54-F8CB-43F8-AF09-BA1DBACED508}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8543432F-0426-4F84-A3DA-A43D3FCBECCF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="690" firstSheet="7" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="690" firstSheet="7" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH2PH" sheetId="17" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3384" uniqueCount="1938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3382" uniqueCount="1937">
   <si>
     <t>Chapter</t>
   </si>
@@ -5672,12 +5672,6 @@
     <t>"pregnancy related mortality ratio"</t>
   </si>
   <si>
-    <t>AM_rates.do</t>
-  </si>
-  <si>
-    <t>AM_gfr</t>
-  </si>
-  <si>
     <t>IR,MR,PR</t>
   </si>
   <si>
@@ -5804,15 +5798,6 @@
     <t>fs_trt_provid</t>
   </si>
   <si>
-    <t>"Provider type among those who sought treatment for fistula"</t>
-  </si>
-  <si>
-    <t>fs_notrt</t>
-  </si>
-  <si>
-    <t>"Did not seek treatmeent for fistula"</t>
-  </si>
-  <si>
     <t>fs_trt_outcome</t>
   </si>
   <si>
@@ -5865,6 +5850,18 @@
   </si>
   <si>
     <t>"Female circumcision type is sewn closed among girls age 0-14"</t>
+  </si>
+  <si>
+    <t>AM_RATES.do</t>
+  </si>
+  <si>
+    <t>AM_GFR.do</t>
+  </si>
+  <si>
+    <t>"Provider type for fistula treatment"</t>
+  </si>
+  <si>
+    <t>FS_FIST.do</t>
   </si>
 </sst>
 </file>
@@ -5954,7 +5951,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5970,12 +5967,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6001,7 +5992,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -6165,7 +6156,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -6514,12 +6504,12 @@
       <c r="B2" s="4" t="s">
         <v>1635</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="61" t="s">
         <v>1636</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -7635,12 +7625,12 @@
       <c r="B2" s="17" t="s">
         <v>1653</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>1654</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
@@ -9135,12 +9125,12 @@
       <c r="B2" s="17" t="s">
         <v>1655</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>1656</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
@@ -9338,7 +9328,7 @@
       <c r="E16" s="17" t="s">
         <v>862</v>
       </c>
-      <c r="F16" s="67" t="s">
+      <c r="F16" s="66" t="s">
         <v>863</v>
       </c>
     </row>
@@ -9352,7 +9342,7 @@
         <v>865</v>
       </c>
       <c r="E17" s="17"/>
-      <c r="F17" s="67"/>
+      <c r="F17" s="66"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="17"/>
@@ -9428,7 +9418,7 @@
       <c r="E23" s="17" t="s">
         <v>805</v>
       </c>
-      <c r="F23" s="68" t="s">
+      <c r="F23" s="67" t="s">
         <v>876</v>
       </c>
     </row>
@@ -9444,7 +9434,7 @@
       <c r="E24" s="17" t="s">
         <v>805</v>
       </c>
-      <c r="F24" s="68"/>
+      <c r="F24" s="67"/>
     </row>
     <row r="25" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
@@ -9458,7 +9448,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="17"/>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="61" t="s">
         <v>880</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -9476,7 +9466,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="17"/>
-      <c r="B27" s="62"/>
+      <c r="B27" s="61"/>
       <c r="C27" s="1" t="s">
         <v>884</v>
       </c>
@@ -9492,7 +9482,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="17"/>
-      <c r="B28" s="62"/>
+      <c r="B28" s="61"/>
       <c r="C28" s="1" t="s">
         <v>886</v>
       </c>
@@ -9508,7 +9498,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="17"/>
-      <c r="B29" s="62"/>
+      <c r="B29" s="61"/>
       <c r="C29" s="17" t="s">
         <v>888</v>
       </c>
@@ -9522,7 +9512,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="17"/>
-      <c r="B30" s="62"/>
+      <c r="B30" s="61"/>
       <c r="C30" s="17" t="s">
         <v>890</v>
       </c>
@@ -9536,7 +9526,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="17"/>
-      <c r="B31" s="62"/>
+      <c r="B31" s="61"/>
       <c r="C31" s="17" t="s">
         <v>892</v>
       </c>
@@ -10148,12 +10138,12 @@
       <c r="B2" s="21" t="s">
         <v>1657</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>1658</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="F3" s="22"/>
@@ -10394,7 +10384,7 @@
       <c r="E26" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="69" t="s">
+      <c r="F26" s="68" t="s">
         <v>974</v>
       </c>
       <c r="G26" s="33"/>
@@ -10409,7 +10399,7 @@
       <c r="E27" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="69"/>
+      <c r="F27" s="68"/>
     </row>
     <row r="28" spans="2:7" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C28" s="24" t="s">
@@ -10421,7 +10411,7 @@
       <c r="E28" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="69"/>
+      <c r="F28" s="68"/>
       <c r="G28" s="33"/>
     </row>
     <row r="29" spans="2:7" s="24" customFormat="1" x14ac:dyDescent="0.35">
@@ -10429,12 +10419,12 @@
         <v>1296</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>1883</v>
+        <v>1881</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="69"/>
+      <c r="F29" s="68"/>
     </row>
     <row r="30" spans="2:7" s="24" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C30" s="24" t="s">
@@ -10935,12 +10925,12 @@
       <c r="B2" s="21" t="s">
         <v>1659</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>1660</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" s="24" t="s">
@@ -10983,7 +10973,7 @@
       <c r="E7" s="24" t="s">
         <v>1019</v>
       </c>
-      <c r="F7" s="69" t="s">
+      <c r="F7" s="68" t="s">
         <v>1020</v>
       </c>
     </row>
@@ -10997,7 +10987,7 @@
       <c r="E8" s="24" t="s">
         <v>1019</v>
       </c>
-      <c r="F8" s="69"/>
+      <c r="F8" s="68"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C9" s="24" t="s">
@@ -11009,7 +10999,7 @@
       <c r="E9" s="24" t="s">
         <v>1019</v>
       </c>
-      <c r="F9" s="69"/>
+      <c r="F9" s="68"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F10" s="41"/>
@@ -11255,12 +11245,12 @@
       <c r="B2" s="21" t="s">
         <v>1661</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>1662</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -11643,7 +11633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -11680,19 +11672,19 @@
       <c r="B2" s="57" t="s">
         <v>1857</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>1663</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C3" s="59"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>1873</v>
+        <v>1933</v>
       </c>
       <c r="C4" t="s">
         <v>1848</v>
@@ -11701,7 +11693,7 @@
         <v>1868</v>
       </c>
       <c r="E4" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -11712,7 +11704,7 @@
         <v>1860</v>
       </c>
       <c r="E5" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -11783,7 +11775,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>1874</v>
+        <v>1934</v>
       </c>
       <c r="C13" t="s">
         <v>1854</v>
@@ -11865,14 +11857,14 @@
         <v>1150</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>1884</v>
-      </c>
-      <c r="C2" s="65" t="s">
+        <v>1882</v>
+      </c>
+      <c r="C2" s="64" t="s">
         <v>1663</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -13252,7 +13244,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D67F9F-843E-495E-AF6B-DD470CD899F4}">
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -13287,27 +13279,27 @@
     </row>
     <row r="2" spans="1:6" s="25" customFormat="1" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
+        <v>1883</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>1884</v>
+      </c>
+      <c r="C2" s="64" t="s">
         <v>1885</v>
       </c>
-      <c r="B2" s="60" t="s">
-        <v>1886</v>
-      </c>
-      <c r="C2" s="65" t="s">
-        <v>1887</v>
-      </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>1932</v>
+        <v>1927</v>
       </c>
       <c r="C4" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
       <c r="D4" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -13315,10 +13307,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C5" s="59" t="s">
-        <v>1891</v>
+        <v>1889</v>
       </c>
       <c r="D5" t="s">
-        <v>1889</v>
+        <v>1887</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -13326,10 +13318,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C6" s="59" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
       <c r="D6" t="s">
-        <v>1894</v>
+        <v>1892</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -13337,10 +13329,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C7" s="59" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
       <c r="D7" t="s">
-        <v>1893</v>
+        <v>1891</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -13348,10 +13340,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C8" s="59" t="s">
-        <v>1904</v>
+        <v>1902</v>
       </c>
       <c r="D8" t="s">
-        <v>1895</v>
+        <v>1893</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -13359,10 +13351,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C9" s="59" t="s">
+        <v>1926</v>
+      </c>
+      <c r="D9" t="s">
         <v>1931</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1936</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -13370,10 +13362,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C10" s="59" t="s">
-        <v>1905</v>
+        <v>1903</v>
       </c>
       <c r="D10" t="s">
-        <v>1926</v>
+        <v>1921</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -13381,10 +13373,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C11" s="59" t="s">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="D11" t="s">
-        <v>1927</v>
+        <v>1922</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -13392,49 +13384,49 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>1933</v>
+        <v>1928</v>
       </c>
       <c r="C13" s="59" t="s">
-        <v>1928</v>
+        <v>1923</v>
       </c>
       <c r="D13" t="s">
-        <v>1934</v>
+        <v>1929</v>
       </c>
       <c r="E13" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C14" s="59" t="s">
-        <v>1929</v>
+        <v>1924</v>
       </c>
       <c r="D14" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
       <c r="E14" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C15" s="59" t="s">
-        <v>1930</v>
+        <v>1925</v>
       </c>
       <c r="D15" t="s">
-        <v>1896</v>
+        <v>1894</v>
       </c>
       <c r="E15" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C16" s="59" t="s">
-        <v>1935</v>
+        <v>1930</v>
       </c>
       <c r="D16" t="s">
-        <v>1937</v>
+        <v>1932</v>
       </c>
       <c r="E16" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.35">
@@ -14215,10 +14207,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{311CF17F-B9D7-4FAE-9BAC-09E565075D78}">
-  <dimension ref="A1:F127"/>
+  <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14252,24 +14244,27 @@
     </row>
     <row r="2" spans="1:6" s="25" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="60" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C2" s="64" t="s">
         <v>1897</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>1936</v>
+      </c>
+      <c r="C4" t="s">
         <v>1898</v>
       </c>
-      <c r="C2" s="65" t="s">
-        <v>1899</v>
-      </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C4" t="s">
-        <v>1900</v>
-      </c>
       <c r="D4" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -14277,10 +14272,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C5" s="35" t="s">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="D5" t="s">
-        <v>1909</v>
+        <v>1907</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -14288,10 +14283,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C6" s="59" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="D6" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -14299,10 +14294,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C8" s="59" t="s">
-        <v>1912</v>
+        <v>1910</v>
       </c>
       <c r="D8" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -14310,10 +14305,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C9" s="59" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="D9" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -14321,10 +14316,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C11" s="59" t="s">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="D11" t="s">
-        <v>1917</v>
+        <v>1935</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -14332,21 +14327,21 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C12" s="59" t="s">
-        <v>1918</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1919</v>
+        <v>1915</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>1916</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C13" s="61" t="s">
-        <v>1920</v>
-      </c>
-      <c r="D13" s="61" t="s">
-        <v>1921</v>
+      <c r="C13" s="59" t="s">
+        <v>1917</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1918</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -14354,33 +14349,25 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C14" s="59" t="s">
-        <v>1922</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1923</v>
+        <v>1919</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>1920</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C15" s="61" t="s">
-        <v>1924</v>
-      </c>
-      <c r="D15" s="61" t="s">
-        <v>1925</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C24" s="35"/>
+      <c r="D24" s="60"/>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C25" s="35"/>
       <c r="D25" s="60"/>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C26" s="35"/>
-      <c r="D26" s="60"/>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B48" s="43"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B49" s="43"/>
@@ -14400,15 +14387,23 @@
     <row r="54" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B54" s="43"/>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B55" s="43"/>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C62" s="59" t="s">
+        <v>1739</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1859</v>
+      </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B63" t="s">
-        <v>1738</v>
-      </c>
       <c r="C63" s="59" t="s">
-        <v>1739</v>
+        <v>1348</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1818</v>
       </c>
       <c r="F63" t="s">
         <v>1859</v>
@@ -14416,10 +14411,10 @@
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C64" s="59" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
       <c r="D64" t="s">
-        <v>1818</v>
+        <v>1819</v>
       </c>
       <c r="F64" t="s">
         <v>1859</v>
@@ -14427,10 +14422,10 @@
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C65" s="59" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
       <c r="D65" t="s">
-        <v>1819</v>
+        <v>1820</v>
       </c>
       <c r="F65" t="s">
         <v>1859</v>
@@ -14438,10 +14433,10 @@
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C66" s="59" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
       <c r="D66" t="s">
-        <v>1820</v>
+        <v>1821</v>
       </c>
       <c r="F66" t="s">
         <v>1859</v>
@@ -14449,10 +14444,10 @@
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C67" s="59" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
       <c r="D67" t="s">
-        <v>1821</v>
+        <v>1822</v>
       </c>
       <c r="F67" t="s">
         <v>1859</v>
@@ -14460,10 +14455,10 @@
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C68" s="59" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="D68" t="s">
-        <v>1822</v>
+        <v>1823</v>
       </c>
       <c r="F68" t="s">
         <v>1859</v>
@@ -14471,10 +14466,10 @@
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C69" s="59" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
       <c r="D69" t="s">
-        <v>1823</v>
+        <v>1824</v>
       </c>
       <c r="F69" t="s">
         <v>1859</v>
@@ -14482,10 +14477,10 @@
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C70" s="59" t="s">
-        <v>1354</v>
+        <v>1740</v>
       </c>
       <c r="D70" t="s">
-        <v>1824</v>
+        <v>1825</v>
       </c>
       <c r="F70" t="s">
         <v>1859</v>
@@ -14493,10 +14488,10 @@
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C71" s="59" t="s">
-        <v>1740</v>
+        <v>1741</v>
       </c>
       <c r="D71" t="s">
-        <v>1825</v>
+        <v>1826</v>
       </c>
       <c r="F71" t="s">
         <v>1859</v>
@@ -14504,10 +14499,10 @@
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C72" s="59" t="s">
-        <v>1741</v>
+        <v>1742</v>
       </c>
       <c r="D72" t="s">
-        <v>1826</v>
+        <v>1827</v>
       </c>
       <c r="F72" t="s">
         <v>1859</v>
@@ -14515,10 +14510,10 @@
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C73" s="59" t="s">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="D73" t="s">
-        <v>1827</v>
+        <v>1828</v>
       </c>
       <c r="F73" t="s">
         <v>1859</v>
@@ -14526,10 +14521,10 @@
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C74" s="59" t="s">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="D74" t="s">
-        <v>1828</v>
+        <v>1829</v>
       </c>
       <c r="F74" t="s">
         <v>1859</v>
@@ -14537,10 +14532,10 @@
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C75" s="59" t="s">
-        <v>1744</v>
+        <v>1355</v>
       </c>
       <c r="D75" t="s">
-        <v>1829</v>
+        <v>1830</v>
       </c>
       <c r="F75" t="s">
         <v>1859</v>
@@ -14548,10 +14543,10 @@
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C76" s="59" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
       <c r="D76" t="s">
-        <v>1830</v>
+        <v>1831</v>
       </c>
       <c r="F76" t="s">
         <v>1859</v>
@@ -14559,10 +14554,10 @@
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C77" s="59" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
       <c r="D77" t="s">
-        <v>1831</v>
+        <v>1832</v>
       </c>
       <c r="F77" t="s">
         <v>1859</v>
@@ -14570,10 +14565,10 @@
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C78" s="59" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D78" t="s">
-        <v>1832</v>
+        <v>1833</v>
       </c>
       <c r="F78" t="s">
         <v>1859</v>
@@ -14581,10 +14576,10 @@
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C79" s="59" t="s">
-        <v>1358</v>
+        <v>1745</v>
       </c>
       <c r="D79" t="s">
-        <v>1833</v>
+        <v>1834</v>
       </c>
       <c r="F79" t="s">
         <v>1859</v>
@@ -14592,10 +14587,10 @@
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C80" s="59" t="s">
-        <v>1745</v>
+        <v>1359</v>
       </c>
       <c r="D80" t="s">
-        <v>1834</v>
+        <v>1835</v>
       </c>
       <c r="F80" t="s">
         <v>1859</v>
@@ -14603,10 +14598,10 @@
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C81" s="59" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
       <c r="D81" t="s">
-        <v>1835</v>
+        <v>1836</v>
       </c>
       <c r="F81" t="s">
         <v>1859</v>
@@ -14614,10 +14609,10 @@
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C82" s="59" t="s">
-        <v>1360</v>
+        <v>1746</v>
       </c>
       <c r="D82" t="s">
-        <v>1836</v>
+        <v>1837</v>
       </c>
       <c r="F82" t="s">
         <v>1859</v>
@@ -14625,10 +14620,10 @@
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C83" s="59" t="s">
-        <v>1746</v>
+        <v>1747</v>
       </c>
       <c r="D83" t="s">
-        <v>1837</v>
+        <v>1838</v>
       </c>
       <c r="F83" t="s">
         <v>1859</v>
@@ -14636,10 +14631,10 @@
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C84" s="59" t="s">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="D84" t="s">
-        <v>1838</v>
+        <v>1839</v>
       </c>
       <c r="F84" t="s">
         <v>1859</v>
@@ -14647,10 +14642,10 @@
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C85" s="59" t="s">
-        <v>1748</v>
+        <v>1749</v>
       </c>
       <c r="D85" t="s">
-        <v>1839</v>
+        <v>1840</v>
       </c>
       <c r="F85" t="s">
         <v>1859</v>
@@ -14658,10 +14653,10 @@
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C86" s="59" t="s">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="D86" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
       <c r="F86" t="s">
         <v>1859</v>
@@ -14669,10 +14664,10 @@
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C87" s="59" t="s">
-        <v>1750</v>
+        <v>1751</v>
       </c>
       <c r="D87" t="s">
-        <v>1841</v>
+        <v>1842</v>
       </c>
       <c r="F87" t="s">
         <v>1859</v>
@@ -14680,10 +14675,10 @@
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C88" s="59" t="s">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="D88" t="s">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="F88" t="s">
         <v>1859</v>
@@ -14691,10 +14686,10 @@
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C89" s="59" t="s">
-        <v>1752</v>
+        <v>1361</v>
       </c>
       <c r="D89" t="s">
-        <v>1843</v>
+        <v>1844</v>
       </c>
       <c r="F89" t="s">
         <v>1859</v>
@@ -14702,10 +14697,10 @@
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C90" s="59" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
       <c r="D90" t="s">
-        <v>1844</v>
+        <v>1845</v>
       </c>
       <c r="F90" t="s">
         <v>1859</v>
@@ -14713,10 +14708,10 @@
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C91" s="59" t="s">
-        <v>1362</v>
+        <v>1753</v>
       </c>
       <c r="D91" t="s">
-        <v>1845</v>
+        <v>1806</v>
       </c>
       <c r="F91" t="s">
         <v>1859</v>
@@ -14724,21 +14719,22 @@
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C92" s="59" t="s">
-        <v>1753</v>
+        <v>1754</v>
       </c>
       <c r="D92" t="s">
-        <v>1806</v>
+        <v>1807</v>
       </c>
       <c r="F92" t="s">
         <v>1859</v>
       </c>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B93" s="43"/>
       <c r="C93" s="59" t="s">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="D93" t="s">
-        <v>1807</v>
+        <v>1808</v>
       </c>
       <c r="F93" t="s">
         <v>1859</v>
@@ -14747,10 +14743,10 @@
     <row r="94" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B94" s="43"/>
       <c r="C94" s="59" t="s">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="D94" t="s">
-        <v>1808</v>
+        <v>1809</v>
       </c>
       <c r="F94" t="s">
         <v>1859</v>
@@ -14759,10 +14755,10 @@
     <row r="95" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B95" s="43"/>
       <c r="C95" s="59" t="s">
-        <v>1756</v>
+        <v>1363</v>
       </c>
       <c r="D95" t="s">
-        <v>1809</v>
+        <v>1811</v>
       </c>
       <c r="F95" t="s">
         <v>1859</v>
@@ -14771,10 +14767,10 @@
     <row r="96" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B96" s="43"/>
       <c r="C96" s="59" t="s">
-        <v>1363</v>
+        <v>1365</v>
       </c>
       <c r="D96" t="s">
-        <v>1811</v>
+        <v>1812</v>
       </c>
       <c r="F96" t="s">
         <v>1859</v>
@@ -14783,10 +14779,10 @@
     <row r="97" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B97" s="43"/>
       <c r="C97" s="59" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
       <c r="D97" t="s">
-        <v>1812</v>
+        <v>1813</v>
       </c>
       <c r="F97" t="s">
         <v>1859</v>
@@ -14795,10 +14791,10 @@
     <row r="98" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B98" s="43"/>
       <c r="C98" s="59" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
       <c r="D98" t="s">
-        <v>1813</v>
+        <v>1814</v>
       </c>
       <c r="F98" t="s">
         <v>1859</v>
@@ -14807,10 +14803,10 @@
     <row r="99" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B99" s="43"/>
       <c r="C99" s="59" t="s">
-        <v>1364</v>
+        <v>1183</v>
       </c>
       <c r="D99" t="s">
-        <v>1814</v>
+        <v>1810</v>
       </c>
       <c r="F99" t="s">
         <v>1859</v>
@@ -14819,10 +14815,10 @@
     <row r="100" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B100" s="43"/>
       <c r="C100" s="59" t="s">
-        <v>1183</v>
+        <v>1757</v>
       </c>
       <c r="D100" t="s">
-        <v>1810</v>
+        <v>1815</v>
       </c>
       <c r="F100" t="s">
         <v>1859</v>
@@ -14831,10 +14827,10 @@
     <row r="101" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B101" s="43"/>
       <c r="C101" s="59" t="s">
-        <v>1757</v>
+        <v>1263</v>
       </c>
       <c r="D101" t="s">
-        <v>1815</v>
+        <v>1184</v>
       </c>
       <c r="F101" t="s">
         <v>1859</v>
@@ -14843,10 +14839,10 @@
     <row r="102" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B102" s="43"/>
       <c r="C102" s="59" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D102" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="F102" t="s">
         <v>1859</v>
@@ -14855,10 +14851,10 @@
     <row r="103" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B103" s="43"/>
       <c r="C103" s="59" t="s">
-        <v>1264</v>
+        <v>1347</v>
       </c>
       <c r="D103" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="F103" t="s">
         <v>1859</v>
@@ -14867,10 +14863,10 @@
     <row r="104" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B104" s="43"/>
       <c r="C104" s="59" t="s">
-        <v>1347</v>
+        <v>1367</v>
       </c>
       <c r="D104" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="F104" t="s">
         <v>1859</v>
@@ -14879,10 +14875,10 @@
     <row r="105" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B105" s="43"/>
       <c r="C105" s="59" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
       <c r="D105" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="F105" t="s">
         <v>1859</v>
@@ -14891,10 +14887,10 @@
     <row r="106" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B106" s="43"/>
       <c r="C106" s="59" t="s">
-        <v>1368</v>
+        <v>1720</v>
       </c>
       <c r="D106" t="s">
-        <v>1188</v>
+        <v>1769</v>
       </c>
       <c r="F106" t="s">
         <v>1859</v>
@@ -14903,10 +14899,10 @@
     <row r="107" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B107" s="43"/>
       <c r="C107" s="59" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="D107" t="s">
-        <v>1769</v>
+        <v>1770</v>
       </c>
       <c r="F107" t="s">
         <v>1859</v>
@@ -14915,10 +14911,10 @@
     <row r="108" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B108" s="43"/>
       <c r="C108" s="59" t="s">
-        <v>1721</v>
+        <v>1758</v>
       </c>
       <c r="D108" t="s">
-        <v>1770</v>
+        <v>1759</v>
       </c>
       <c r="F108" t="s">
         <v>1859</v>
@@ -14927,33 +14923,33 @@
     <row r="109" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B109" s="43"/>
       <c r="C109" s="59" t="s">
-        <v>1758</v>
+        <v>1722</v>
       </c>
       <c r="D109" t="s">
-        <v>1759</v>
+        <v>1771</v>
       </c>
       <c r="F109" t="s">
         <v>1859</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B110" s="43"/>
       <c r="C110" s="59" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="D110" t="s">
-        <v>1771</v>
+        <v>1772</v>
       </c>
       <c r="F110" t="s">
         <v>1859</v>
       </c>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B111" s="6"/>
       <c r="C111" s="59" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="D111" t="s">
-        <v>1772</v>
+        <v>1773</v>
       </c>
       <c r="F111" t="s">
         <v>1859</v>
@@ -14962,10 +14958,10 @@
     <row r="112" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B112" s="6"/>
       <c r="C112" s="59" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="D112" t="s">
-        <v>1773</v>
+        <v>1774</v>
       </c>
       <c r="F112" t="s">
         <v>1859</v>
@@ -14974,10 +14970,10 @@
     <row r="113" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B113" s="6"/>
       <c r="C113" s="59" t="s">
-        <v>1725</v>
+        <v>1760</v>
       </c>
       <c r="D113" t="s">
-        <v>1774</v>
+        <v>1816</v>
       </c>
       <c r="F113" t="s">
         <v>1859</v>
@@ -14986,10 +14982,10 @@
     <row r="114" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B114" s="6"/>
       <c r="C114" s="59" t="s">
-        <v>1760</v>
+        <v>1761</v>
       </c>
       <c r="D114" t="s">
-        <v>1816</v>
+        <v>1733</v>
       </c>
       <c r="F114" t="s">
         <v>1859</v>
@@ -14998,10 +14994,10 @@
     <row r="115" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B115" s="6"/>
       <c r="C115" s="59" t="s">
-        <v>1761</v>
+        <v>1762</v>
       </c>
       <c r="D115" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
       <c r="F115" t="s">
         <v>1859</v>
@@ -15010,10 +15006,10 @@
     <row r="116" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B116" s="6"/>
       <c r="C116" s="59" t="s">
-        <v>1762</v>
+        <v>1763</v>
       </c>
       <c r="D116" t="s">
-        <v>1731</v>
+        <v>1729</v>
       </c>
       <c r="F116" t="s">
         <v>1859</v>
@@ -15022,10 +15018,10 @@
     <row r="117" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B117" s="6"/>
       <c r="C117" s="59" t="s">
-        <v>1763</v>
+        <v>1764</v>
       </c>
       <c r="D117" t="s">
-        <v>1729</v>
+        <v>1817</v>
       </c>
       <c r="F117" t="s">
         <v>1859</v>
@@ -15033,28 +15029,28 @@
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B118" s="6"/>
-      <c r="C118" s="59" t="s">
-        <v>1764</v>
-      </c>
-      <c r="D118" t="s">
-        <v>1817</v>
-      </c>
-      <c r="F118" t="s">
-        <v>1859</v>
-      </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B119" s="6"/>
+      <c r="B119" s="6" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C119" s="59" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D119" t="s">
+        <v>1177</v>
+      </c>
+      <c r="F119" t="s">
+        <v>1859</v>
+      </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B120" s="6" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C120" s="59" t="s">
-        <v>1257</v>
+      <c r="B120" s="6"/>
+      <c r="C120" t="s">
+        <v>1258</v>
       </c>
       <c r="D120" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="F120" t="s">
         <v>1859</v>
@@ -15063,10 +15059,10 @@
     <row r="121" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B121" s="6"/>
       <c r="C121" t="s">
-        <v>1258</v>
+        <v>1261</v>
       </c>
       <c r="D121" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="F121" t="s">
         <v>1859</v>
@@ -15075,10 +15071,10 @@
     <row r="122" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B122" s="6"/>
       <c r="C122" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="D122" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="F122" t="s">
         <v>1859</v>
@@ -15087,10 +15083,10 @@
     <row r="123" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B123" s="6"/>
       <c r="C123" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
       <c r="D123" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="F123" t="s">
         <v>1859</v>
@@ -15099,22 +15095,21 @@
     <row r="124" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B124" s="6"/>
       <c r="C124" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D124" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="F124" t="s">
         <v>1859</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B125" s="6"/>
       <c r="C125" t="s">
-        <v>1260</v>
+        <v>1846</v>
       </c>
       <c r="D125" t="s">
-        <v>1182</v>
+        <v>1714</v>
       </c>
       <c r="F125" t="s">
         <v>1859</v>
@@ -15122,23 +15117,12 @@
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C126" t="s">
-        <v>1846</v>
+        <v>1847</v>
       </c>
       <c r="D126" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="F126" t="s">
-        <v>1859</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="C127" t="s">
-        <v>1847</v>
-      </c>
-      <c r="D127" t="s">
-        <v>1713</v>
-      </c>
-      <c r="F127" t="s">
         <v>1859</v>
       </c>
     </row>
@@ -15196,12 +15180,12 @@
       <c r="B2" s="4" t="s">
         <v>1637</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="61" t="s">
         <v>1638</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -15750,12 +15734,12 @@
       <c r="B2" s="4" t="s">
         <v>1639</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="61" t="s">
         <v>1640</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -16140,12 +16124,12 @@
       <c r="B2" s="5" t="s">
         <v>1641</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="63" t="s">
         <v>1642</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
@@ -16312,7 +16296,7 @@
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>1664</v>
@@ -16338,10 +16322,10 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>63</v>
@@ -16357,10 +16341,10 @@
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
-        <v>1879</v>
+        <v>1877</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>53</v>
@@ -16373,10 +16357,10 @@
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
-        <v>1881</v>
+        <v>1879</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>1882</v>
+        <v>1880</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>53</v>
@@ -16889,12 +16873,12 @@
       <c r="B2" s="5" t="s">
         <v>1643</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="63" t="s">
         <v>1644</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
@@ -17088,12 +17072,12 @@
       <c r="B2" s="17" t="s">
         <v>1645</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>1646</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="17"/>
@@ -17463,7 +17447,7 @@
       <c r="E29" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F29" s="65" t="s">
+      <c r="F29" s="64" t="s">
         <v>161</v>
       </c>
     </row>
@@ -17479,7 +17463,7 @@
       <c r="E30" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="65"/>
+      <c r="F30" s="64"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="17"/>
@@ -17493,7 +17477,7 @@
       <c r="E31" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F31" s="65"/>
+      <c r="F31" s="64"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="17"/>
@@ -17507,7 +17491,7 @@
       <c r="E32" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="65"/>
+      <c r="F32" s="64"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="17"/>
@@ -17521,7 +17505,7 @@
       <c r="E33" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="65"/>
+      <c r="F33" s="64"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="17"/>
@@ -17535,7 +17519,7 @@
       <c r="E34" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="65"/>
+      <c r="F34" s="64"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="17"/>
@@ -17549,7 +17533,7 @@
       <c r="E35" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="65"/>
+      <c r="F35" s="64"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="17"/>
@@ -17563,7 +17547,7 @@
       <c r="E36" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="65"/>
+      <c r="F36" s="64"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="17"/>
@@ -17577,7 +17561,7 @@
       <c r="E37" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="65"/>
+      <c r="F37" s="64"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="17"/>
@@ -17591,7 +17575,7 @@
       <c r="E38" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="65"/>
+      <c r="F38" s="64"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="17"/>
@@ -17605,7 +17589,7 @@
       <c r="E39" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="65"/>
+      <c r="F39" s="64"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="17"/>
@@ -17619,7 +17603,7 @@
       <c r="E40" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="65"/>
+      <c r="F40" s="64"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="17"/>
@@ -17633,7 +17617,7 @@
       <c r="E41" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F41" s="65"/>
+      <c r="F41" s="64"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="17"/>
@@ -17647,7 +17631,7 @@
       <c r="E42" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="65"/>
+      <c r="F42" s="64"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="17"/>
@@ -17661,7 +17645,7 @@
       <c r="E43" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="65"/>
+      <c r="F43" s="64"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="17"/>
@@ -17675,7 +17659,7 @@
       <c r="E44" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F44" s="65"/>
+      <c r="F44" s="64"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="17"/>
@@ -17689,7 +17673,7 @@
       <c r="E45" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="65"/>
+      <c r="F45" s="64"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="17"/>
@@ -17703,7 +17687,7 @@
       <c r="E46" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="65"/>
+      <c r="F46" s="64"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="17"/>
@@ -18235,7 +18219,7 @@
       <c r="E86" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F86" s="65" t="s">
+      <c r="F86" s="64" t="s">
         <v>267</v>
       </c>
     </row>
@@ -18251,7 +18235,7 @@
       <c r="E87" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F87" s="65"/>
+      <c r="F87" s="64"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="17"/>
@@ -18265,7 +18249,7 @@
       <c r="E88" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F88" s="65"/>
+      <c r="F88" s="64"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="17"/>
@@ -18279,7 +18263,7 @@
       <c r="E89" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F89" s="65"/>
+      <c r="F89" s="64"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="17"/>
@@ -18293,7 +18277,7 @@
       <c r="E90" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F90" s="65"/>
+      <c r="F90" s="64"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="17"/>
@@ -18307,7 +18291,7 @@
       <c r="E91" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F91" s="65"/>
+      <c r="F91" s="64"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="17"/>
@@ -18321,7 +18305,7 @@
       <c r="E92" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F92" s="65"/>
+      <c r="F92" s="64"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="17"/>
@@ -18335,7 +18319,7 @@
       <c r="E93" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F93" s="65"/>
+      <c r="F93" s="64"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="17"/>
@@ -18349,7 +18333,7 @@
       <c r="E94" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F94" s="65"/>
+      <c r="F94" s="64"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="17"/>
@@ -18363,7 +18347,7 @@
       <c r="E95" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F95" s="65"/>
+      <c r="F95" s="64"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="17"/>
@@ -18377,7 +18361,7 @@
       <c r="E96" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F96" s="65"/>
+      <c r="F96" s="64"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="17"/>
@@ -18391,7 +18375,7 @@
       <c r="E97" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F97" s="65"/>
+      <c r="F97" s="64"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="17"/>
@@ -18405,7 +18389,7 @@
       <c r="E98" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F98" s="65"/>
+      <c r="F98" s="64"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="17"/>
@@ -18419,7 +18403,7 @@
       <c r="E99" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F99" s="65"/>
+      <c r="F99" s="64"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="17"/>
@@ -19004,7 +18988,7 @@
       </c>
       <c r="F143" s="17"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A144" s="17"/>
       <c r="B144" s="17"/>
       <c r="C144" s="17" t="s">
@@ -19094,12 +19078,12 @@
       <c r="B2" s="5" t="s">
         <v>1647</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="63" t="s">
         <v>1648</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
@@ -19114,10 +19098,10 @@
       <c r="B4" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="C4" s="66" t="s">
+      <c r="C4" s="65" t="s">
         <v>379</v>
       </c>
-      <c r="D4" s="66"/>
+      <c r="D4" s="65"/>
       <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
@@ -19856,12 +19840,12 @@
       <c r="B2" s="17" t="s">
         <v>1649</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>1650</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="17"/>
@@ -20499,12 +20483,12 @@
       <c r="B2" s="17" t="s">
         <v>1651</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="C2" s="64" t="s">
         <v>1652</v>
       </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="17"/>
@@ -22105,7 +22089,7 @@
       <c r="E123" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="F123" s="65" t="s">
+      <c r="F123" s="64" t="s">
         <v>1041</v>
       </c>
     </row>
@@ -22121,7 +22105,7 @@
       <c r="E124" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="F124" s="65"/>
+      <c r="F124" s="64"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="17"/>
@@ -22157,30 +22141,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Survey_x0020_Type xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">DHS</Survey_x0020_Type>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-6680</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">
-      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-6680</Url>
-      <Description>VMX3MACP777Z-432858100-6680</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="533" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9fe6dd6fbc47b2b2c3033f1a9c1079fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd9e5a0c56088652e9b5d1a36fcd7f8a" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -22449,6 +22409,30 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Survey_x0020_Type xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">DHS</Survey_x0020_Type>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-6680</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">
+      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-6680</Url>
+      <Description>VMX3MACP777Z-432858100-6680</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
@@ -22500,9 +22484,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90E9E434-4B8B-4BAE-8E0F-2B34F42316A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8D26296-6F3A-450E-9A4D-26E32036C996}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
+    <ds:schemaRef ds:uri="d16efad5-0601-4cf0-b7c2-89968258c777"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22526,21 +22522,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8D26296-6F3A-450E-9A4D-26E32036C996}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90E9E434-4B8B-4BAE-8E0F-2B34F42316A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
-    <ds:schemaRef ds:uri="d16efad5-0601-4cf0-b7c2-89968258c777"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
DHS8 update Chapter 3 - RC
DHS8 updates to Respondent characteristics Chapter
</commit_message>
<xml_diff>
--- a/IndicatorList.xlsx
+++ b/IndicatorList.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/Shared Resources/Code/DHS-Indicators-Stata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{D5F216C4-D72E-4091-BD40-86EC314E3642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8F8ADEC-A67D-4595-935B-C8E85729B1CB}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{D5F216C4-D72E-4091-BD40-86EC314E3642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{814064B8-358B-4DE1-96AB-37EC9CE7A0EF}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1755" windowWidth="29040" windowHeight="15840" tabRatio="690" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45120" yWindow="-4530" windowWidth="16440" windowHeight="28440" tabRatio="690" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH2PH" sheetId="17" r:id="rId1"/>
-    <sheet name="CH3RC" sheetId="16" r:id="rId2"/>
+    <sheet name="CH3RC" sheetId="24" r:id="rId2"/>
     <sheet name="Ch4MS" sheetId="2" r:id="rId3"/>
     <sheet name="Ch5FE" sheetId="3" r:id="rId4"/>
     <sheet name="Ch6FF" sheetId="4" r:id="rId5"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4018" uniqueCount="2266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4046" uniqueCount="2280">
   <si>
     <t>Chapter</t>
   </si>
@@ -6853,6 +6853,48 @@
   </si>
   <si>
     <t>"HepB at birth vaccination according to either source"</t>
+  </si>
+  <si>
+    <t>rc_alc_any</t>
+  </si>
+  <si>
+    <t>"Consumed alcohol in the last one month"</t>
+  </si>
+  <si>
+    <t>rc_alc_freq</t>
+  </si>
+  <si>
+    <t>"Frequency of drinking among those who consumed alcohol in the last one month"</t>
+  </si>
+  <si>
+    <t>rc_alc_drinks</t>
+  </si>
+  <si>
+    <t>"Average number of drinks consumed among those who consumed alcohol in the last one month"</t>
+  </si>
+  <si>
+    <t>rc_place_birth</t>
+  </si>
+  <si>
+    <t>"Place of birth and residence"</t>
+  </si>
+  <si>
+    <t>rc_migrant_5yrs</t>
+  </si>
+  <si>
+    <t>"Migrant that moved to current place of residence in the last 5 years"</t>
+  </si>
+  <si>
+    <t>rc_migrant_type</t>
+  </si>
+  <si>
+    <t>"Type of migrant that moved to current place of residence in the last 5 years"</t>
+  </si>
+  <si>
+    <t>rc_migrant_reason</t>
+  </si>
+  <si>
+    <t>"Reason for migration among those who moved to current place of residence in the last 5 years"</t>
   </si>
 </sst>
 </file>
@@ -7094,8 +7136,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -17168,11 +17210,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9131FEDA-1CF1-4CA8-9871-E8FF10DC2924}">
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17180,7 +17222,7 @@
     <col min="1" max="1" width="16.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="71.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.453125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.81640625" style="1"/>
@@ -17274,7 +17316,7 @@
       </c>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15" t="s">
@@ -17291,25 +17333,19 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="15" t="s">
-        <v>1135</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>1140</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="15"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>9</v>
@@ -17320,10 +17356,10 @@
       <c r="A10" s="15"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>9</v>
@@ -17334,24 +17370,24 @@
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>9</v>
@@ -17362,10 +17398,10 @@
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15" t="s">
-        <v>1010</v>
+        <v>1139</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>1011</v>
+        <v>1144</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>9</v>
@@ -17376,24 +17412,24 @@
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>9</v>
@@ -17404,66 +17440,60 @@
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>1145</v>
+        <v>1015</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="15"/>
     </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
-      <c r="C17" s="15" t="s">
-        <v>1017</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>1018</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>1022</v>
+        <v>1145</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="15"/>
     </row>
-    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="15"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>1023</v>
+        <v>1018</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>9</v>
@@ -17474,52 +17504,46 @@
       <c r="A21" s="15"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15" t="s">
-        <v>1146</v>
+        <v>1020</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>1151</v>
+        <v>1023</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="15"/>
     </row>
-    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15" t="s">
-        <v>1167</v>
+        <v>1021</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>1147</v>
+        <v>1024</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="15"/>
     </row>
-    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
-      <c r="C23" s="15" t="s">
-        <v>1168</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>1148</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="15"/>
     </row>
-    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15" t="s">
-        <v>1169</v>
+        <v>1146</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>1149</v>
+        <v>1151</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>9</v>
@@ -17530,10 +17554,10 @@
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>9</v>
@@ -17544,10 +17568,10 @@
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15" t="s">
-        <v>1025</v>
+        <v>1168</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>1026</v>
+        <v>1148</v>
       </c>
       <c r="E26" s="15" t="s">
         <v>9</v>
@@ -17558,10 +17582,10 @@
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15" t="s">
-        <v>1027</v>
+        <v>1169</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>1028</v>
+        <v>1149</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>9</v>
@@ -17572,10 +17596,10 @@
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15" t="s">
-        <v>1029</v>
+        <v>1170</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>1030</v>
+        <v>1150</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>9</v>
@@ -17586,10 +17610,10 @@
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15" t="s">
-        <v>1165</v>
+        <v>1025</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>1166</v>
+        <v>1026</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>9</v>
@@ -17599,28 +17623,22 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
-      <c r="C30" s="15" t="s">
-        <v>1032</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>1033</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
       <c r="F30" s="15"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15" t="s">
-        <v>1034</v>
+        <v>1027</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>1035</v>
+        <v>1028</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F31" s="15"/>
     </row>
@@ -17628,10 +17646,10 @@
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15" t="s">
-        <v>1152</v>
+        <v>1029</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>1158</v>
+        <v>1030</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>9</v>
@@ -17642,10 +17660,10 @@
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15" t="s">
-        <v>1153</v>
+        <v>1165</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>1159</v>
+        <v>1166</v>
       </c>
       <c r="E33" s="15" t="s">
         <v>9</v>
@@ -17656,13 +17674,13 @@
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15" t="s">
-        <v>1154</v>
+        <v>1032</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>1161</v>
+        <v>1033</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F34" s="15"/>
     </row>
@@ -17670,47 +17688,201 @@
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15" t="s">
-        <v>1155</v>
+        <v>1034</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>1160</v>
+        <v>1035</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F35" s="15"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C36" s="1" t="s">
-        <v>1157</v>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15" t="s">
+        <v>1152</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
       <c r="E36" s="15" t="s">
         <v>9</v>
       </c>
+      <c r="F36" s="15"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C37" s="1" t="s">
-        <v>1156</v>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15" t="s">
+        <v>1153</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>9</v>
       </c>
+      <c r="F37" s="15"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C38" s="1" t="s">
-        <v>1031</v>
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15" t="s">
+        <v>1154</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="E38" s="15" t="s">
         <v>9</v>
+      </c>
+      <c r="F38" s="15"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="15"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C40" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C41" s="1" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C42" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C44" s="1" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>2267</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C45" s="1" t="s">
+        <v>2268</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>2269</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C46" s="1" t="s">
+        <v>2270</v>
+      </c>
+      <c r="D46" s="37" t="s">
+        <v>2271</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C48" s="1" t="s">
+        <v>2272</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>2273</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C49" s="1" t="s">
+        <v>2274</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>2275</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C50" s="1" t="s">
+        <v>2276</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>2277</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="C51" s="1" t="s">
+        <v>2278</v>
+      </c>
+      <c r="D51" s="37" t="s">
+        <v>2279</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>1861</v>
       </c>
     </row>
   </sheetData>
@@ -23247,8 +23419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C48DB349-AD5D-467C-98A6-AE80A94E1333}">
   <dimension ref="A1:F169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView topLeftCell="A96" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24089,13 +24261,13 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="15"/>
       <c r="B63" s="15"/>
-      <c r="C63" s="37" t="s">
+      <c r="C63" s="15" t="s">
         <v>2253</v>
       </c>
-      <c r="D63" s="37" t="s">
+      <c r="D63" s="15" t="s">
         <v>2254</v>
       </c>
-      <c r="E63" s="37" t="s">
+      <c r="E63" s="15" t="s">
         <v>73</v>
       </c>
       <c r="F63" s="15" t="s">
@@ -24105,13 +24277,13 @@
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
-      <c r="C64" s="37" t="s">
+      <c r="C64" s="15" t="s">
         <v>2256</v>
       </c>
-      <c r="D64" s="37" t="s">
+      <c r="D64" s="15" t="s">
         <v>2257</v>
       </c>
-      <c r="E64" s="37" t="s">
+      <c r="E64" s="15" t="s">
         <v>73</v>
       </c>
       <c r="F64" s="15" t="s">
@@ -24121,13 +24293,13 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="15"/>
       <c r="B65" s="15"/>
-      <c r="C65" s="37" t="s">
+      <c r="C65" s="15" t="s">
         <v>2258</v>
       </c>
-      <c r="D65" s="37" t="s">
+      <c r="D65" s="15" t="s">
         <v>2259</v>
       </c>
-      <c r="E65" s="37" t="s">
+      <c r="E65" s="15" t="s">
         <v>73</v>
       </c>
       <c r="F65" s="15" t="s">
@@ -24137,21 +24309,21 @@
     <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="15"/>
       <c r="B66" s="15"/>
-      <c r="C66" s="37"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
       <c r="F66" s="15"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="15"/>
       <c r="B67" s="15"/>
-      <c r="C67" s="37" t="s">
+      <c r="C67" s="15" t="s">
         <v>2260</v>
       </c>
-      <c r="D67" s="37" t="s">
+      <c r="D67" s="15" t="s">
         <v>2261</v>
       </c>
-      <c r="E67" s="37" t="s">
+      <c r="E67" s="15" t="s">
         <v>73</v>
       </c>
       <c r="F67" s="15" t="s">
@@ -24161,13 +24333,13 @@
     <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="15"/>
       <c r="B68" s="15"/>
-      <c r="C68" s="37" t="s">
+      <c r="C68" s="15" t="s">
         <v>2262</v>
       </c>
-      <c r="D68" s="37" t="s">
+      <c r="D68" s="15" t="s">
         <v>2263</v>
       </c>
-      <c r="E68" s="37" t="s">
+      <c r="E68" s="15" t="s">
         <v>73</v>
       </c>
       <c r="F68" s="15" t="s">
@@ -24177,13 +24349,13 @@
     <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="15"/>
       <c r="B69" s="15"/>
-      <c r="C69" s="37" t="s">
+      <c r="C69" s="15" t="s">
         <v>2264</v>
       </c>
-      <c r="D69" s="37" t="s">
+      <c r="D69" s="15" t="s">
         <v>2265</v>
       </c>
-      <c r="E69" s="37" t="s">
+      <c r="E69" s="15" t="s">
         <v>73</v>
       </c>
       <c r="F69" s="15" t="s">
@@ -25605,6 +25777,84 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Survey_x0020_Type xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">DHS</Survey_x0020_Type>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-6680</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">
+      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-6680</Url>
+      <Description>VMX3MACP777Z-432858100-6680</Description>
+    </_dlc_DocIdUrl>
+    <TaxCatchAll xmlns="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="537" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="32af978db1d8a110ec558ab40ef27856">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" xmlns:ns4="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="490a248aacda82af6307d667c2e14f68" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25904,85 +26154,42 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC59F560-844B-432B-8AD6-73714CEDFB96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
+    <ds:schemaRef ds:uri="d16efad5-0601-4cf0-b7c2-89968258c777"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90E9E434-4B8B-4BAE-8E0F-2B34F42316A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Survey_x0020_Type xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">DHS</Survey_x0020_Type>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-6680</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">
-      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-6680</Url>
-      <Description>VMX3MACP777Z-432858100-6680</Description>
-    </_dlc_DocIdUrl>
-    <TaxCatchAll xmlns="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C070FFD4-2B81-40A9-9526-59DD893E6C18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7400C4A1-7880-4671-9CBA-143AD7B24860}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26001,39 +26208,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C070FFD4-2B81-40A9-9526-59DD893E6C18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90E9E434-4B8B-4BAE-8E0F-2B34F42316A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC59F560-844B-432B-8AD6-73714CEDFB96}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
-    <ds:schemaRef ds:uri="d16efad5-0601-4cf0-b7c2-89968258c777"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DHS8 update Chapter 4 - MS
DHS8 updates to Marriage & Sexual Activity Chapter
</commit_message>
<xml_diff>
--- a/IndicatorList.xlsx
+++ b/IndicatorList.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/Shared Resources/Code/DHS-Indicators-Stata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{D5F216C4-D72E-4091-BD40-86EC314E3642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{814064B8-358B-4DE1-96AB-37EC9CE7A0EF}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{D5F216C4-D72E-4091-BD40-86EC314E3642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E30737ED-297F-407F-A3D1-800905074644}"/>
   <bookViews>
-    <workbookView xWindow="-45120" yWindow="-4530" windowWidth="16440" windowHeight="28440" tabRatio="690" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1755" windowWidth="29040" windowHeight="15840" tabRatio="690" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH2PH" sheetId="17" r:id="rId1"/>
     <sheet name="CH3RC" sheetId="24" r:id="rId2"/>
-    <sheet name="Ch4MS" sheetId="2" r:id="rId3"/>
+    <sheet name="Ch4MS" sheetId="25" r:id="rId3"/>
     <sheet name="Ch5FE" sheetId="3" r:id="rId4"/>
     <sheet name="Ch6FF" sheetId="4" r:id="rId5"/>
     <sheet name="Ch7FP" sheetId="20" r:id="rId6"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4046" uniqueCount="2280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4062" uniqueCount="2288">
   <si>
     <t>Chapter</t>
   </si>
@@ -6895,6 +6895,30 @@
   </si>
   <si>
     <t>"Reason for migration among those who moved to current place of residence in the last 5 years"</t>
+  </si>
+  <si>
+    <t>ms_mar_regis</t>
+  </si>
+  <si>
+    <t>"Current marriage is registered with civil authorities"</t>
+  </si>
+  <si>
+    <t>ms_mar_doc</t>
+  </si>
+  <si>
+    <t>"Current marriage is registered and has documentation recognizing the marriage/union"</t>
+  </si>
+  <si>
+    <t>ms_mar_cert</t>
+  </si>
+  <si>
+    <t>"Current marriage is registered and has a marriage certificate"</t>
+  </si>
+  <si>
+    <t>ms_sex_timing</t>
+  </si>
+  <si>
+    <t>"Timing of recent sexual activity"</t>
   </si>
 </sst>
 </file>
@@ -7036,7 +7060,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -7116,6 +7140,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7136,8 +7163,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7463,12 +7490,12 @@
       <c r="B2" s="4" t="s">
         <v>1536</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="31" t="s">
         <v>1537</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -8585,12 +8612,12 @@
       <c r="B2" s="15" t="s">
         <v>1554</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>1970</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
@@ -11270,12 +11297,12 @@
       <c r="B2" s="15" t="s">
         <v>1555</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>1556</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
@@ -11473,7 +11500,7 @@
       <c r="E16" s="15" t="s">
         <v>809</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="36" t="s">
         <v>810</v>
       </c>
     </row>
@@ -11487,7 +11514,7 @@
         <v>812</v>
       </c>
       <c r="E17" s="15"/>
-      <c r="F17" s="35"/>
+      <c r="F17" s="36"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="15"/>
@@ -11563,7 +11590,7 @@
       <c r="E23" s="15" t="s">
         <v>752</v>
       </c>
-      <c r="F23" s="36" t="s">
+      <c r="F23" s="37" t="s">
         <v>823</v>
       </c>
     </row>
@@ -11579,7 +11606,7 @@
       <c r="E24" s="15" t="s">
         <v>752</v>
       </c>
-      <c r="F24" s="36"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
@@ -11593,7 +11620,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="15"/>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="31" t="s">
         <v>827</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -11611,7 +11638,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="15"/>
-      <c r="B27" s="30"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="1" t="s">
         <v>831</v>
       </c>
@@ -11627,7 +11654,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="15"/>
-      <c r="B28" s="30"/>
+      <c r="B28" s="31"/>
       <c r="C28" s="1" t="s">
         <v>833</v>
       </c>
@@ -11643,7 +11670,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="15"/>
-      <c r="B29" s="30"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="15" t="s">
         <v>835</v>
       </c>
@@ -11657,7 +11684,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
-      <c r="B30" s="30"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="15" t="s">
         <v>837</v>
       </c>
@@ -11671,7 +11698,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="15"/>
-      <c r="B31" s="30"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="15" t="s">
         <v>839</v>
       </c>
@@ -12283,12 +12310,12 @@
       <c r="B2" s="15" t="s">
         <v>1557</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>1558</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="F3" s="5"/>
@@ -12529,7 +12556,7 @@
       <c r="E26" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="32" t="s">
+      <c r="F26" s="33" t="s">
         <v>921</v>
       </c>
       <c r="G26" s="21"/>
@@ -12544,7 +12571,7 @@
       <c r="E27" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="32"/>
+      <c r="F27" s="33"/>
     </row>
     <row r="28" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C28" s="18" t="s">
@@ -12556,7 +12583,7 @@
       <c r="E28" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="32"/>
+      <c r="F28" s="33"/>
       <c r="G28" s="21"/>
     </row>
     <row r="29" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.35">
@@ -12569,7 +12596,7 @@
       <c r="E29" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="32"/>
+      <c r="F29" s="33"/>
     </row>
     <row r="30" spans="2:7" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C30" s="18" t="s">
@@ -13070,12 +13097,12 @@
       <c r="B2" s="15" t="s">
         <v>1559</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>1560</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" s="18" t="s">
@@ -13118,7 +13145,7 @@
       <c r="E7" s="18" t="s">
         <v>966</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="33" t="s">
         <v>967</v>
       </c>
     </row>
@@ -13132,7 +13159,7 @@
       <c r="E8" s="18" t="s">
         <v>966</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C9" s="18" t="s">
@@ -13144,7 +13171,7 @@
       <c r="E9" s="18" t="s">
         <v>966</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C11" s="18" t="s">
@@ -13368,12 +13395,12 @@
       <c r="B2" s="15" t="s">
         <v>1561</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>1562</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -13795,12 +13822,12 @@
       <c r="B2" s="15" t="s">
         <v>1757</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>1563</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -13979,12 +14006,12 @@
       <c r="B2" s="15" t="s">
         <v>1782</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>1563</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -15389,12 +15416,12 @@
       <c r="B2" s="15" t="s">
         <v>1784</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>1785</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -16339,12 +16366,12 @@
       <c r="B2" s="15" t="s">
         <v>1796</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>1797</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -17213,7 +17240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9131FEDA-1CF1-4CA8-9871-E8FF10DC2924}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
@@ -17255,12 +17282,12 @@
       <c r="B2" s="4" t="s">
         <v>1538</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="31" t="s">
         <v>1539</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -17819,7 +17846,7 @@
       <c r="C46" s="1" t="s">
         <v>2270</v>
       </c>
-      <c r="D46" s="37" t="s">
+      <c r="D46" s="30" t="s">
         <v>2271</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -17875,7 +17902,7 @@
       <c r="C51" s="1" t="s">
         <v>2278</v>
       </c>
-      <c r="D51" s="37" t="s">
+      <c r="D51" s="30" t="s">
         <v>2279</v>
       </c>
       <c r="E51" s="1" t="s">
@@ -17894,11 +17921,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D9FD1F-9E04-40FA-B90D-BB6D8A41E98B}">
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17906,7 +17933,7 @@
     <col min="1" max="1" width="16.453125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="58.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.453125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.81640625" style="1"/>
@@ -17939,12 +17966,12 @@
       <c r="B2" s="4" t="s">
         <v>1540</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="31" t="s">
         <v>1541</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -17987,292 +18014,348 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="15"/>
       <c r="B6" s="15"/>
-      <c r="C6" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="15" t="s">
+      <c r="C6" s="38" t="s">
+        <v>2280</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>2281</v>
+      </c>
+      <c r="E6" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F6" s="38" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="15" t="s">
+      <c r="C7" s="38" t="s">
+        <v>2282</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>2283</v>
+      </c>
+      <c r="E7" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="38" t="s">
+        <v>1861</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
-      <c r="C8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="15"/>
+      <c r="C8" s="38" t="s">
+        <v>2284</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>2285</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>1861</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="15"/>
       <c r="B9" s="15"/>
-      <c r="C9" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="15"/>
+      <c r="C9" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="15"/>
       <c r="B10" s="15"/>
-      <c r="C10" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="15"/>
+      <c r="C10" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="38"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="15"/>
+      <c r="C11" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="15" t="s">
+      <c r="C12" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="15"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="15" t="s">
+      <c r="C13" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
-      <c r="C14" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="15" t="s">
+      <c r="C14" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="15"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
-      <c r="C15" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="15" t="s">
+      <c r="C15" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="15" t="s">
-        <v>34</v>
-      </c>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
-      <c r="C16" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="15" t="s">
+      <c r="C16" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="15"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="15"/>
       <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="38"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="15"/>
-      <c r="B18" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="15" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="15"/>
+      <c r="F18" s="38" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="15"/>
       <c r="B19" s="15"/>
-      <c r="C19" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="15" t="s">
+      <c r="C19" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="15"/>
+      <c r="F19" s="38"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="15"/>
       <c r="B20" s="15"/>
-      <c r="C20" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="15" t="s">
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="15"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="15"/>
+      <c r="F21" s="38"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
-      <c r="C22" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="15" t="s">
+      <c r="C22" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="15"/>
-    </row>
-    <row r="23" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="F22" s="38"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="15"/>
       <c r="B23" s="15"/>
-      <c r="C23" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="15" t="s">
+      <c r="C23" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="15" t="s">
-        <v>34</v>
-      </c>
+      <c r="F23" s="38"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
-      <c r="C24" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="15" t="s">
+      <c r="C24" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="38"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
+      <c r="C25" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="15"/>
       <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
+      <c r="C26" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="38" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+      <c r="C27" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="38"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="38" t="s">
+        <v>2286</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>2287</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="38" t="s">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -18328,12 +18411,12 @@
       <c r="B2" s="5" t="s">
         <v>1542</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="33" t="s">
         <v>1543</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
@@ -19077,12 +19160,12 @@
       <c r="B2" s="5" t="s">
         <v>1544</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="33" t="s">
         <v>1545</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
@@ -19276,12 +19359,12 @@
       <c r="B2" s="15" t="s">
         <v>1546</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>1547</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
@@ -19673,7 +19756,7 @@
       <c r="E31" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="34" t="s">
         <v>1856</v>
       </c>
     </row>
@@ -19689,7 +19772,7 @@
       <c r="E32" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="15"/>
@@ -19703,7 +19786,7 @@
       <c r="E33" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F33" s="33"/>
+      <c r="F33" s="34"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="15"/>
@@ -19717,7 +19800,7 @@
       <c r="E34" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="33"/>
+      <c r="F34" s="34"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="15"/>
@@ -19731,7 +19814,7 @@
       <c r="E35" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F35" s="33"/>
+      <c r="F35" s="34"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="15"/>
@@ -19745,7 +19828,7 @@
       <c r="E36" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F36" s="33"/>
+      <c r="F36" s="34"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="15"/>
@@ -19759,7 +19842,7 @@
       <c r="E37" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="33"/>
+      <c r="F37" s="34"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="15"/>
@@ -19773,7 +19856,7 @@
       <c r="E38" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F38" s="33"/>
+      <c r="F38" s="34"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="15"/>
@@ -19787,7 +19870,7 @@
       <c r="E39" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F39" s="33"/>
+      <c r="F39" s="34"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="15"/>
@@ -19801,7 +19884,7 @@
       <c r="E40" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F40" s="33"/>
+      <c r="F40" s="34"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="15"/>
@@ -19815,7 +19898,7 @@
       <c r="E41" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F41" s="33"/>
+      <c r="F41" s="34"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="15"/>
@@ -19829,7 +19912,7 @@
       <c r="E42" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="33"/>
+      <c r="F42" s="34"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="15"/>
@@ -19843,7 +19926,7 @@
       <c r="E43" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="33"/>
+      <c r="F43" s="34"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="15"/>
@@ -19857,7 +19940,7 @@
       <c r="E44" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F44" s="33"/>
+      <c r="F44" s="34"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="15"/>
@@ -19871,7 +19954,7 @@
       <c r="E45" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F45" s="33"/>
+      <c r="F45" s="34"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="15"/>
@@ -19885,7 +19968,7 @@
       <c r="E46" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F46" s="33"/>
+      <c r="F46" s="34"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="15"/>
@@ -19899,7 +19982,7 @@
       <c r="E47" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F47" s="33"/>
+      <c r="F47" s="34"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="15"/>
@@ -19913,7 +19996,7 @@
       <c r="E48" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F48" s="33"/>
+      <c r="F48" s="34"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="15"/>
@@ -20533,7 +20616,7 @@
       <c r="E94" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F94" s="33" t="s">
+      <c r="F94" s="34" t="s">
         <v>265</v>
       </c>
     </row>
@@ -20549,7 +20632,7 @@
       <c r="E95" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F95" s="33"/>
+      <c r="F95" s="34"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="15"/>
@@ -20563,7 +20646,7 @@
       <c r="E96" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F96" s="33"/>
+      <c r="F96" s="34"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="15"/>
@@ -20577,7 +20660,7 @@
       <c r="E97" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F97" s="33"/>
+      <c r="F97" s="34"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="15"/>
@@ -20591,7 +20674,7 @@
       <c r="E98" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F98" s="33"/>
+      <c r="F98" s="34"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="15"/>
@@ -20605,7 +20688,7 @@
       <c r="E99" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F99" s="33"/>
+      <c r="F99" s="34"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="15"/>
@@ -20619,7 +20702,7 @@
       <c r="E100" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F100" s="33"/>
+      <c r="F100" s="34"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="15"/>
@@ -20633,7 +20716,7 @@
       <c r="E101" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F101" s="33"/>
+      <c r="F101" s="34"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="15"/>
@@ -20647,7 +20730,7 @@
       <c r="E102" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F102" s="33"/>
+      <c r="F102" s="34"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="15"/>
@@ -20661,7 +20744,7 @@
       <c r="E103" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F103" s="33"/>
+      <c r="F103" s="34"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="15"/>
@@ -20675,7 +20758,7 @@
       <c r="E104" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F104" s="33"/>
+      <c r="F104" s="34"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="15"/>
@@ -20689,7 +20772,7 @@
       <c r="E105" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F105" s="33"/>
+      <c r="F105" s="34"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="15"/>
@@ -20703,7 +20786,7 @@
       <c r="E106" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F106" s="33"/>
+      <c r="F106" s="34"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="15"/>
@@ -20717,7 +20800,7 @@
       <c r="E107" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F107" s="33"/>
+      <c r="F107" s="34"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="15"/>
@@ -21533,12 +21616,12 @@
       <c r="B2" s="5" t="s">
         <v>1548</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="33" t="s">
         <v>1549</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
@@ -21553,10 +21636,10 @@
       <c r="B4" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="35" t="s">
         <v>374</v>
       </c>
-      <c r="D4" s="34"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
@@ -22295,12 +22378,12 @@
       <c r="B2" s="15" t="s">
         <v>1550</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>1551</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
@@ -23461,12 +23544,12 @@
       <c r="B2" s="15" t="s">
         <v>1552</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>1553</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="15"/>
@@ -25777,84 +25860,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Survey_x0020_Type xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">DHS</Survey_x0020_Type>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-6680</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">
-      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-6680</Url>
-      <Description>VMX3MACP777Z-432858100-6680</Description>
-    </_dlc_DocIdUrl>
-    <TaxCatchAll xmlns="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="537" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="32af978db1d8a110ec558ab40ef27856">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" xmlns:ns4="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="490a248aacda82af6307d667c2e14f68" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -26154,42 +26159,85 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC59F560-844B-432B-8AD6-73714CEDFB96}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
-    <ds:schemaRef ds:uri="d16efad5-0601-4cf0-b7c2-89968258c777"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90E9E434-4B8B-4BAE-8E0F-2B34F42316A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C070FFD4-2B81-40A9-9526-59DD893E6C18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Survey_x0020_Type xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">DHS</Survey_x0020_Type>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-6680</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">
+      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-6680</Url>
+      <Description>VMX3MACP777Z-432858100-6680</Description>
+    </_dlc_DocIdUrl>
+    <TaxCatchAll xmlns="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7400C4A1-7880-4671-9CBA-143AD7B24860}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26208,4 +26256,39 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C070FFD4-2B81-40A9-9526-59DD893E6C18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90E9E434-4B8B-4BAE-8E0F-2B34F42316A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC59F560-844B-432B-8AD6-73714CEDFB96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
+    <ds:schemaRef ds:uri="d16efad5-0601-4cf0-b7c2-89968258c777"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="fa6a9aea-fb0f-4ddd-aff8-712634b7d5fe"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>